<commit_message>
don't cache - use the workbook to retrieve sheets, rows, cells
</commit_message>
<xml_diff>
--- a/output/fluentmanyrows.xlsx
+++ b/output/fluentmanyrows.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="198">
   <si>
     <t>Name</t>
   </si>
@@ -23,598 +23,589 @@
     <t>Hired</t>
   </si>
   <si>
-    <t>Ronnie Stark</t>
-  </si>
-  <si>
-    <t>Central Legal Manager</t>
-  </si>
-  <si>
-    <t>Lawrence Nicolas Jr.</t>
-  </si>
-  <si>
-    <t>National Executive</t>
-  </si>
-  <si>
-    <t>Miss Wynell Moen</t>
-  </si>
-  <si>
-    <t>Accounting Architect</t>
-  </si>
-  <si>
-    <t>Rodney Hickle DDS</t>
-  </si>
-  <si>
-    <t>Advertising Strategist</t>
-  </si>
-  <si>
-    <t>Otis Heller DVM</t>
-  </si>
-  <si>
-    <t>Legal Supervisor</t>
-  </si>
-  <si>
-    <t>Silvia Schaefer</t>
-  </si>
-  <si>
-    <t>Direct Technology Consultant</t>
-  </si>
-  <si>
-    <t>Sima Fay</t>
-  </si>
-  <si>
-    <t>Dynamic Design Representative</t>
-  </si>
-  <si>
-    <t>Wade Dicki</t>
-  </si>
-  <si>
-    <t>Forward Banking Analyst</t>
-  </si>
-  <si>
-    <t>Temple Herzog II</t>
-  </si>
-  <si>
-    <t>Real-Estate Liaison</t>
-  </si>
-  <si>
-    <t>Hayden Crist</t>
-  </si>
-  <si>
-    <t>Real-Estate Developer</t>
-  </si>
-  <si>
-    <t>Corrinne Morissette</t>
-  </si>
-  <si>
-    <t>Internal IT Specialist</t>
-  </si>
-  <si>
-    <t>Ms. Delmar Klein</t>
-  </si>
-  <si>
-    <t>Legacy Associate</t>
-  </si>
-  <si>
-    <t>Mr. Hayden Kuhlman</t>
-  </si>
-  <si>
-    <t>Advertising Orchestrator</t>
-  </si>
-  <si>
-    <t>Nisha Koelpin Sr.</t>
-  </si>
-  <si>
-    <t>Central Hospitality Developer</t>
-  </si>
-  <si>
-    <t>Rayford Swaniawski</t>
-  </si>
-  <si>
-    <t>Internal Consultant</t>
-  </si>
-  <si>
-    <t>Caroll Kilback</t>
-  </si>
-  <si>
-    <t>Product Facilitator</t>
-  </si>
-  <si>
-    <t>Kanesha Mertz</t>
-  </si>
-  <si>
-    <t>Sales Director</t>
-  </si>
-  <si>
-    <t>Frederick Sanford</t>
-  </si>
-  <si>
-    <t>Sales Associate</t>
-  </si>
-  <si>
-    <t>Dreama Corkery</t>
-  </si>
-  <si>
-    <t>Corporate Technology Developer</t>
-  </si>
-  <si>
-    <t>Dr. Latrice Hane</t>
-  </si>
-  <si>
-    <t>Retail Administrator</t>
-  </si>
-  <si>
-    <t>Yong Schumm</t>
-  </si>
-  <si>
-    <t>Human Coordinator</t>
-  </si>
-  <si>
-    <t>Domingo McLaughlin</t>
-  </si>
-  <si>
-    <t>Forward Orchestrator</t>
-  </si>
-  <si>
-    <t>Forrest Konopelski</t>
-  </si>
-  <si>
-    <t>Senior Mining Planner</t>
-  </si>
-  <si>
-    <t>Arlen Homenick</t>
-  </si>
-  <si>
-    <t>Sales Specialist</t>
-  </si>
-  <si>
-    <t>Tennie Witting</t>
-  </si>
-  <si>
-    <t>Marketing Consultant</t>
-  </si>
-  <si>
-    <t>Cory Stokes</t>
-  </si>
-  <si>
-    <t>Lead Advertising Architect</t>
-  </si>
-  <si>
-    <t>Joya Morissette</t>
-  </si>
-  <si>
-    <t>International Liaison</t>
-  </si>
-  <si>
-    <t>German Trantow</t>
-  </si>
-  <si>
-    <t>Corporate Construction Liaison</t>
-  </si>
-  <si>
-    <t>Darrell Marks IV</t>
-  </si>
-  <si>
-    <t>Construction Architect</t>
-  </si>
-  <si>
-    <t>Mrs. Alica Kunze</t>
-  </si>
-  <si>
-    <t>Internal Marketing Facilitator</t>
-  </si>
-  <si>
-    <t>Mr. Alfredo Roob</t>
-  </si>
-  <si>
-    <t>Forward Planner</t>
-  </si>
-  <si>
-    <t>Tory Kuhic</t>
-  </si>
-  <si>
-    <t>Senior Accounting Agent</t>
-  </si>
-  <si>
-    <t>Mrs. Bernie Conroy</t>
-  </si>
-  <si>
-    <t>Forward Assistant</t>
-  </si>
-  <si>
-    <t>Scottie Parker Sr.</t>
-  </si>
-  <si>
-    <t>Accounting Strategist</t>
-  </si>
-  <si>
-    <t>Lyla Emard</t>
-  </si>
-  <si>
-    <t>Marketing Analyst</t>
-  </si>
-  <si>
-    <t>Angelo Hackett</t>
-  </si>
-  <si>
-    <t>Global Strategist</t>
-  </si>
-  <si>
-    <t>Roman Bins</t>
-  </si>
-  <si>
-    <t>Healthcare Officer</t>
-  </si>
-  <si>
-    <t>Janey Corwin MD</t>
-  </si>
-  <si>
-    <t>Principal Facilitator</t>
-  </si>
-  <si>
-    <t>Latoya Lakin</t>
-  </si>
-  <si>
-    <t>Construction Associate</t>
-  </si>
-  <si>
-    <t>Mr. Louie Waelchi</t>
-  </si>
-  <si>
-    <t>Customer Director</t>
-  </si>
-  <si>
-    <t>Allison Jacobson</t>
-  </si>
-  <si>
-    <t>Consulting Coordinator</t>
-  </si>
-  <si>
-    <t>Filomena Hayes</t>
+    <t>Jackie Beatty</t>
+  </si>
+  <si>
+    <t>Direct Farming Designer</t>
+  </si>
+  <si>
+    <t>Len Kirlin II</t>
+  </si>
+  <si>
+    <t>Direct Agent</t>
+  </si>
+  <si>
+    <t>Delta Dicki</t>
+  </si>
+  <si>
+    <t>Forward Hospitality Producer</t>
+  </si>
+  <si>
+    <t>Samara Ernser</t>
+  </si>
+  <si>
+    <t>Technology Executive</t>
+  </si>
+  <si>
+    <t>Lucinda Reynolds</t>
+  </si>
+  <si>
+    <t>Human Legal Liaison</t>
+  </si>
+  <si>
+    <t>Allegra Schamberger</t>
+  </si>
+  <si>
+    <t>Forward Retail Administrator</t>
+  </si>
+  <si>
+    <t>Tegan Harvey</t>
+  </si>
+  <si>
+    <t>Internal Designer</t>
+  </si>
+  <si>
+    <t>Mr. Inez Ziemann</t>
+  </si>
+  <si>
+    <t>Marketing Associate</t>
+  </si>
+  <si>
+    <t>Karine Dibbert</t>
+  </si>
+  <si>
+    <t>National Advertising Associate</t>
+  </si>
+  <si>
+    <t>Guadalupe Jast</t>
+  </si>
+  <si>
+    <t>Human Architect</t>
+  </si>
+  <si>
+    <t>Donn Goodwin</t>
+  </si>
+  <si>
+    <t>International Technology Specialist</t>
+  </si>
+  <si>
+    <t>Elijah Paucek</t>
+  </si>
+  <si>
+    <t>Future Design Coordinator</t>
+  </si>
+  <si>
+    <t>Willian Treutel</t>
+  </si>
+  <si>
+    <t>Customer Orchestrator</t>
+  </si>
+  <si>
+    <t>Alberto Ernser</t>
+  </si>
+  <si>
+    <t>Administration Supervisor</t>
+  </si>
+  <si>
+    <t>Drucilla Wintheiser</t>
+  </si>
+  <si>
+    <t>Dynamic Facilitator</t>
+  </si>
+  <si>
+    <t>Annalee Carter</t>
+  </si>
+  <si>
+    <t>Corporate Administrator</t>
+  </si>
+  <si>
+    <t>Grant Veum</t>
+  </si>
+  <si>
+    <t>Real-Estate Administrator</t>
+  </si>
+  <si>
+    <t>Mrs. Mohammed Waters</t>
+  </si>
+  <si>
+    <t>Technology Assistant</t>
+  </si>
+  <si>
+    <t>Tory Kertzmann</t>
+  </si>
+  <si>
+    <t>Advertising Director</t>
+  </si>
+  <si>
+    <t>Mr. Jolynn Greenfelder</t>
+  </si>
+  <si>
+    <t>Legacy Sales Associate</t>
+  </si>
+  <si>
+    <t>Miss Georgia Nienow</t>
+  </si>
+  <si>
+    <t>Banking Consultant</t>
+  </si>
+  <si>
+    <t>Hermine Wisoky</t>
+  </si>
+  <si>
+    <t>Principal Accounting Associate</t>
+  </si>
+  <si>
+    <t>Marvella Blanda</t>
+  </si>
+  <si>
+    <t>Human Manufacturing Designer</t>
+  </si>
+  <si>
+    <t>Jesse Turcotte I</t>
+  </si>
+  <si>
+    <t>Regional Education Supervisor</t>
+  </si>
+  <si>
+    <t>Odette Barton</t>
+  </si>
+  <si>
+    <t>Design Specialist</t>
+  </si>
+  <si>
+    <t>Israel Konopelski V</t>
+  </si>
+  <si>
+    <t>Internal Design Orchestrator</t>
+  </si>
+  <si>
+    <t>Damion VonRueden</t>
+  </si>
+  <si>
+    <t>Chief Technician</t>
+  </si>
+  <si>
+    <t>Wesley Klocko</t>
+  </si>
+  <si>
+    <t>Legacy Producer</t>
+  </si>
+  <si>
+    <t>Norah Dickens II</t>
+  </si>
+  <si>
+    <t>Community-Services Executive</t>
+  </si>
+  <si>
+    <t>David Bailey</t>
+  </si>
+  <si>
+    <t>Senior Consultant</t>
+  </si>
+  <si>
+    <t>Delmer Hilll</t>
+  </si>
+  <si>
+    <t>Regional Legal Officer</t>
+  </si>
+  <si>
+    <t>Jim Lynch</t>
+  </si>
+  <si>
+    <t>Investor Analyst</t>
+  </si>
+  <si>
+    <t>Mr. Leigh Hodkiewicz</t>
+  </si>
+  <si>
+    <t>Customer Accounting Facilitator</t>
+  </si>
+  <si>
+    <t>Dawn Walsh</t>
+  </si>
+  <si>
+    <t>Miss Ceola Parisian</t>
+  </si>
+  <si>
+    <t>Global Construction Administrator</t>
+  </si>
+  <si>
+    <t>Mrs. Georgeanna Ledner</t>
+  </si>
+  <si>
+    <t>Future IT Manager</t>
+  </si>
+  <si>
+    <t>Ethan Adams</t>
+  </si>
+  <si>
+    <t>Legacy Government Coordinator</t>
+  </si>
+  <si>
+    <t>Donald Kuphal PhD</t>
+  </si>
+  <si>
+    <t>Design Liaison</t>
+  </si>
+  <si>
+    <t>Eusebio Kuhn DDS</t>
+  </si>
+  <si>
+    <t>Legal Strategist</t>
+  </si>
+  <si>
+    <t>Bret Keeling</t>
+  </si>
+  <si>
+    <t>Direct Advertising Supervisor</t>
+  </si>
+  <si>
+    <t>Dr. Derick Zemlak</t>
+  </si>
+  <si>
+    <t>Manufacturing Executive</t>
+  </si>
+  <si>
+    <t>Colton Harris</t>
+  </si>
+  <si>
+    <t>Investor Banking Orchestrator</t>
+  </si>
+  <si>
+    <t>Hong Reinger</t>
+  </si>
+  <si>
+    <t>National Accounting Agent</t>
+  </si>
+  <si>
+    <t>Alan Reynolds PhD</t>
+  </si>
+  <si>
+    <t>Chief Farming Coordinator</t>
+  </si>
+  <si>
+    <t>Dr. Ethelyn Mills</t>
+  </si>
+  <si>
+    <t>Marketing Manager</t>
+  </si>
+  <si>
+    <t>Nickolas Anderson</t>
+  </si>
+  <si>
+    <t>Banking Liaison</t>
+  </si>
+  <si>
+    <t>Caryn Brown</t>
+  </si>
+  <si>
+    <t>Real-Estate Associate</t>
+  </si>
+  <si>
+    <t>Bud Heidenreich</t>
+  </si>
+  <si>
+    <t>Legal Coordinator</t>
+  </si>
+  <si>
+    <t>Williams Schaden</t>
+  </si>
+  <si>
+    <t>Destiny Gutmann</t>
+  </si>
+  <si>
+    <t>Principal Developer</t>
+  </si>
+  <si>
+    <t>Mr. Houston Franecki</t>
   </si>
   <si>
     <t>Hospitality Orchestrator</t>
   </si>
   <si>
-    <t>Bradford Weber Jr.</t>
-  </si>
-  <si>
-    <t>Forward Legal Architect</t>
-  </si>
-  <si>
-    <t>Bari Batz</t>
-  </si>
-  <si>
-    <t>Mining Facilitator</t>
-  </si>
-  <si>
-    <t>Ms. Dusti Hayes</t>
-  </si>
-  <si>
-    <t>Legal Engineer</t>
-  </si>
-  <si>
-    <t>Virgil Fisher</t>
-  </si>
-  <si>
-    <t>Hospitality Consultant</t>
-  </si>
-  <si>
-    <t>Zofia Friesen</t>
-  </si>
-  <si>
-    <t>Education Developer</t>
-  </si>
-  <si>
-    <t>Ty Murphy V</t>
-  </si>
-  <si>
-    <t>Senior Banking Manager</t>
-  </si>
-  <si>
-    <t>Claudio Tremblay</t>
-  </si>
-  <si>
-    <t>International Engineer</t>
-  </si>
-  <si>
-    <t>Fernanda Bogisich</t>
-  </si>
-  <si>
-    <t>Miss Tamra Cronin</t>
-  </si>
-  <si>
-    <t>Internal Community-Services Developer</t>
-  </si>
-  <si>
-    <t>Gerald Gottlieb</t>
-  </si>
-  <si>
-    <t>District Representative</t>
-  </si>
-  <si>
-    <t>Damian Block</t>
-  </si>
-  <si>
-    <t>Manufacturing Officer</t>
-  </si>
-  <si>
-    <t>Royal Jones</t>
+    <t>Vergie Dickens</t>
+  </si>
+  <si>
+    <t>Legacy Farming Manager</t>
+  </si>
+  <si>
+    <t>Henry Douglas</t>
+  </si>
+  <si>
+    <t>Product Marketing Director</t>
+  </si>
+  <si>
+    <t>Sherita Collins</t>
+  </si>
+  <si>
+    <t>Senior Legal Manager</t>
+  </si>
+  <si>
+    <t>Isreal Hackett II</t>
+  </si>
+  <si>
+    <t>Accounting Designer</t>
+  </si>
+  <si>
+    <t>Arline Kulas</t>
+  </si>
+  <si>
+    <t>Regional Consulting Officer</t>
+  </si>
+  <si>
+    <t>Neal Bradtke</t>
+  </si>
+  <si>
+    <t>Technology Agent</t>
+  </si>
+  <si>
+    <t>Roxanna Howell I</t>
+  </si>
+  <si>
+    <t>Investor Government Liaison</t>
+  </si>
+  <si>
+    <t>Bryon Yost</t>
+  </si>
+  <si>
+    <t>Regional Mining Planner</t>
+  </si>
+  <si>
+    <t>Mrs. Dani Rosenbaum</t>
   </si>
   <si>
     <t>Accounting Analyst</t>
   </si>
   <si>
-    <t>Desmond Weimann</t>
-  </si>
-  <si>
-    <t>Lead Marketing Manager</t>
-  </si>
-  <si>
-    <t>Jay Lindgren</t>
-  </si>
-  <si>
-    <t>Corporate Technology Architect</t>
-  </si>
-  <si>
-    <t>Hank Kling</t>
-  </si>
-  <si>
-    <t>National Government Associate</t>
-  </si>
-  <si>
-    <t>Wayne Kertzmann</t>
-  </si>
-  <si>
-    <t>Community-Services Planner</t>
-  </si>
-  <si>
-    <t>Ms. Wilson Ward</t>
-  </si>
-  <si>
-    <t>Ralph Hettinger</t>
-  </si>
-  <si>
-    <t>Marketing Manager</t>
-  </si>
-  <si>
-    <t>Burt McDermott</t>
-  </si>
-  <si>
-    <t>IT Coordinator</t>
-  </si>
-  <si>
-    <t>Paulene Quigley PhD</t>
-  </si>
-  <si>
-    <t>Direct Representative</t>
-  </si>
-  <si>
-    <t>Maire Wunsch</t>
-  </si>
-  <si>
-    <t>Human Legal Consultant</t>
-  </si>
-  <si>
-    <t>Rogelio Pfeffer</t>
-  </si>
-  <si>
-    <t>Investor Liaison</t>
-  </si>
-  <si>
-    <t>Winifred Waters</t>
-  </si>
-  <si>
-    <t>International Hospitality Strategist</t>
-  </si>
-  <si>
-    <t>Dr. Librada Koelpin</t>
-  </si>
-  <si>
-    <t>Mining Agent</t>
-  </si>
-  <si>
-    <t>Ms. Arthur Stamm</t>
+    <t>Veta Rohan</t>
+  </si>
+  <si>
+    <t>Consulting Facilitator</t>
+  </si>
+  <si>
+    <t>Jeannine McLaughlin</t>
+  </si>
+  <si>
+    <t>Investor Agent</t>
+  </si>
+  <si>
+    <t>Jaimee Abernathy</t>
+  </si>
+  <si>
+    <t>Consulting Executive</t>
+  </si>
+  <si>
+    <t>Tamika Stanton</t>
+  </si>
+  <si>
+    <t>Dynamic Supervisor</t>
+  </si>
+  <si>
+    <t>Lesha Welch</t>
+  </si>
+  <si>
+    <t>National Farming Assistant</t>
+  </si>
+  <si>
+    <t>Ms. Linwood Cummings</t>
+  </si>
+  <si>
+    <t>Corporate Facilitator</t>
+  </si>
+  <si>
+    <t>Chi Terry Jr.</t>
+  </si>
+  <si>
+    <t>Central Officer</t>
+  </si>
+  <si>
+    <t>Lieselotte Marvin</t>
+  </si>
+  <si>
+    <t>Administration Administrator</t>
+  </si>
+  <si>
+    <t>Loretta O'Connell</t>
+  </si>
+  <si>
+    <t>Mining Representative</t>
+  </si>
+  <si>
+    <t>Roseline Parker</t>
+  </si>
+  <si>
+    <t>Mining Analyst</t>
+  </si>
+  <si>
+    <t>Allyn Orn I</t>
+  </si>
+  <si>
+    <t>Central Director</t>
+  </si>
+  <si>
+    <t>Britt O'Connell</t>
+  </si>
+  <si>
+    <t>Central Agent</t>
+  </si>
+  <si>
+    <t>Gearldine Gottlieb</t>
   </si>
   <si>
     <t>Education Coordinator</t>
   </si>
   <si>
-    <t>Monique Collier</t>
-  </si>
-  <si>
-    <t>Customer Specialist</t>
-  </si>
-  <si>
-    <t>Denny Schimmel</t>
-  </si>
-  <si>
-    <t>Real-Estate Consultant</t>
-  </si>
-  <si>
-    <t>Shelton Zulauf</t>
-  </si>
-  <si>
-    <t>International Coordinator</t>
-  </si>
-  <si>
-    <t>Kathi Altenwerth</t>
-  </si>
-  <si>
-    <t>Mining Developer</t>
-  </si>
-  <si>
-    <t>Michael Runte</t>
-  </si>
-  <si>
-    <t>International Administration Assistant</t>
-  </si>
-  <si>
-    <t>Irena Funk</t>
-  </si>
-  <si>
-    <t>Forward Developer</t>
-  </si>
-  <si>
-    <t>Arie Goldner DDS</t>
-  </si>
-  <si>
-    <t>Chief Representative</t>
-  </si>
-  <si>
-    <t>Miss Vicente Walker</t>
-  </si>
-  <si>
-    <t>Direct Executive</t>
-  </si>
-  <si>
-    <t>Miss Kylee Macejkovic</t>
-  </si>
-  <si>
-    <t>Accounting Developer</t>
-  </si>
-  <si>
-    <t>Stanley Botsford DDS</t>
-  </si>
-  <si>
-    <t>Central Marketing Developer</t>
-  </si>
-  <si>
-    <t>Kasey Mertz</t>
-  </si>
-  <si>
-    <t>Product Technology Producer</t>
-  </si>
-  <si>
-    <t>Damaris Ryan</t>
-  </si>
-  <si>
-    <t>Legal Orchestrator</t>
-  </si>
-  <si>
-    <t>Ezekiel Abshire</t>
-  </si>
-  <si>
-    <t>International Consultant</t>
-  </si>
-  <si>
-    <t>Galen Corkery</t>
-  </si>
-  <si>
-    <t>District Officer</t>
-  </si>
-  <si>
-    <t>Gayle Keeling</t>
-  </si>
-  <si>
-    <t>Sales Coordinator</t>
-  </si>
-  <si>
-    <t>Ricarda Leuschke Sr.</t>
-  </si>
-  <si>
-    <t>District Administrator</t>
-  </si>
-  <si>
-    <t>Garrett Shanahan</t>
-  </si>
-  <si>
-    <t>Technology Officer</t>
-  </si>
-  <si>
-    <t>Nia Dicki I</t>
-  </si>
-  <si>
-    <t>Legal Planner</t>
-  </si>
-  <si>
-    <t>Ester Erdman</t>
-  </si>
-  <si>
-    <t>Government Officer</t>
-  </si>
-  <si>
-    <t>Tod Doyle DVM</t>
-  </si>
-  <si>
-    <t>IT Analyst</t>
-  </si>
-  <si>
-    <t>Darren Osinski V</t>
-  </si>
-  <si>
-    <t>Farming Analyst</t>
-  </si>
-  <si>
-    <t>Dwight Satterfield</t>
-  </si>
-  <si>
-    <t>Human Associate</t>
-  </si>
-  <si>
-    <t>Rob Hackett</t>
-  </si>
-  <si>
-    <t>Design Engineer</t>
-  </si>
-  <si>
-    <t>Zora Carroll</t>
-  </si>
-  <si>
-    <t>Marketing Strategist</t>
-  </si>
-  <si>
-    <t>Trey Rodriguez</t>
-  </si>
-  <si>
-    <t>Legal Agent</t>
-  </si>
-  <si>
-    <t>Freddie Huel</t>
-  </si>
-  <si>
-    <t>Corporate Assistant</t>
-  </si>
-  <si>
-    <t>Irmgard Zboncak IV</t>
-  </si>
-  <si>
-    <t>Accounting Executive</t>
-  </si>
-  <si>
-    <t>Tim Lebsack</t>
-  </si>
-  <si>
-    <t>District Advertising Executive</t>
-  </si>
-  <si>
-    <t>Sanora Harvey</t>
-  </si>
-  <si>
-    <t>Sales Architect</t>
-  </si>
-  <si>
-    <t>Bobbie Mohr II</t>
-  </si>
-  <si>
-    <t>Direct Community-Services Administrator</t>
-  </si>
-  <si>
-    <t>Lyman Hyatt III</t>
-  </si>
-  <si>
-    <t>Administration Analyst</t>
-  </si>
-  <si>
-    <t>Herbert McGlynn</t>
-  </si>
-  <si>
-    <t>Manufacturing Executive</t>
-  </si>
-  <si>
-    <t>Abe VonRueden</t>
-  </si>
-  <si>
-    <t>Corporate Specialist</t>
+    <t>Corina Beer</t>
+  </si>
+  <si>
+    <t>Hospitality Engineer</t>
+  </si>
+  <si>
+    <t>Delbert Jacobs V</t>
+  </si>
+  <si>
+    <t>Dynamic Design Producer</t>
+  </si>
+  <si>
+    <t>Christen Rau</t>
+  </si>
+  <si>
+    <t>National Supervisor</t>
+  </si>
+  <si>
+    <t>Internal Architect</t>
+  </si>
+  <si>
+    <t>Larry Ruecker</t>
+  </si>
+  <si>
+    <t>Dynamic Manufacturing Engineer</t>
+  </si>
+  <si>
+    <t>Vasiliki Larson</t>
+  </si>
+  <si>
+    <t>Future Advertising Representative</t>
+  </si>
+  <si>
+    <t>Lisbeth Reinger</t>
+  </si>
+  <si>
+    <t>Hilton Kertzmann</t>
+  </si>
+  <si>
+    <t>Legacy Real-Estate Liaison</t>
+  </si>
+  <si>
+    <t>Catrice Prohaska</t>
+  </si>
+  <si>
+    <t>Principal Representative</t>
+  </si>
+  <si>
+    <t>Tess Breitenberg</t>
+  </si>
+  <si>
+    <t>Regional Accounting Strategist</t>
+  </si>
+  <si>
+    <t>Doretta Hilll</t>
+  </si>
+  <si>
+    <t>District Banking Orchestrator</t>
+  </si>
+  <si>
+    <t>Octavio Lowe</t>
+  </si>
+  <si>
+    <t>Regional Orchestrator</t>
+  </si>
+  <si>
+    <t>Dominique Trantow</t>
+  </si>
+  <si>
+    <t>Cherri Torp</t>
+  </si>
+  <si>
+    <t>National Consultant</t>
+  </si>
+  <si>
+    <t>Joe Harvey</t>
+  </si>
+  <si>
+    <t>Investor Retail Liaison</t>
+  </si>
+  <si>
+    <t>Lakeesha Jacobs</t>
+  </si>
+  <si>
+    <t>Forward Design Consultant</t>
+  </si>
+  <si>
+    <t>Miss Josef Bailey</t>
+  </si>
+  <si>
+    <t>Customer Accounting Technician</t>
+  </si>
+  <si>
+    <t>Jasmin Shields</t>
+  </si>
+  <si>
+    <t>Corporate Education Architect</t>
+  </si>
+  <si>
+    <t>Odis Cassin</t>
+  </si>
+  <si>
+    <t>Mining Architect</t>
+  </si>
+  <si>
+    <t>Sheldon Gusikowski</t>
+  </si>
+  <si>
+    <t>Senior Officer</t>
+  </si>
+  <si>
+    <t>Henrietta Prosacco</t>
+  </si>
+  <si>
+    <t>Customer Assistant</t>
+  </si>
+  <si>
+    <t>Harvey Nicolas</t>
+  </si>
+  <si>
+    <t>Global Associate</t>
+  </si>
+  <si>
+    <t>Willard Morar</t>
+  </si>
+  <si>
+    <t>Customer Consultant</t>
+  </si>
+  <si>
+    <t>Willena Walker</t>
+  </si>
+  <si>
+    <t>Legal Representative</t>
+  </si>
+  <si>
+    <t>Dr. Augustine Johns</t>
+  </si>
+  <si>
+    <t>Senior Executive</t>
+  </si>
+  <si>
+    <t>Scot Cronin</t>
+  </si>
+  <si>
+    <t>Farming Orchestrator</t>
+  </si>
+  <si>
+    <t>Dorene Stroman</t>
+  </si>
+  <si>
+    <t>Product Manager</t>
   </si>
 </sst>
 </file>
@@ -1047,7 +1038,7 @@
         <v>69</v>
       </c>
       <c r="B35" t="s">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="C35" t="n" s="1">
         <v>44339.0</v>
@@ -1055,10 +1046,10 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36" t="s">
         <v>71</v>
-      </c>
-      <c r="B36" t="s">
-        <v>72</v>
       </c>
       <c r="C36" t="n" s="1">
         <v>44346.0</v>
@@ -1066,10 +1057,10 @@
     </row>
     <row r="37">
       <c r="A37" t="s">
+        <v>72</v>
+      </c>
+      <c r="B37" t="s">
         <v>73</v>
-      </c>
-      <c r="B37" t="s">
-        <v>74</v>
       </c>
       <c r="C37" t="n" s="1">
         <v>44353.0</v>
@@ -1077,10 +1068,10 @@
     </row>
     <row r="38">
       <c r="A38" t="s">
+        <v>74</v>
+      </c>
+      <c r="B38" t="s">
         <v>75</v>
-      </c>
-      <c r="B38" t="s">
-        <v>76</v>
       </c>
       <c r="C38" t="n" s="1">
         <v>44360.0</v>
@@ -1088,10 +1079,10 @@
     </row>
     <row r="39">
       <c r="A39" t="s">
+        <v>76</v>
+      </c>
+      <c r="B39" t="s">
         <v>77</v>
-      </c>
-      <c r="B39" t="s">
-        <v>78</v>
       </c>
       <c r="C39" t="n" s="1">
         <v>44367.0</v>
@@ -1099,10 +1090,10 @@
     </row>
     <row r="40">
       <c r="A40" t="s">
+        <v>78</v>
+      </c>
+      <c r="B40" t="s">
         <v>79</v>
-      </c>
-      <c r="B40" t="s">
-        <v>80</v>
       </c>
       <c r="C40" t="n" s="1">
         <v>44374.0</v>
@@ -1110,10 +1101,10 @@
     </row>
     <row r="41">
       <c r="A41" t="s">
+        <v>80</v>
+      </c>
+      <c r="B41" t="s">
         <v>81</v>
-      </c>
-      <c r="B41" t="s">
-        <v>82</v>
       </c>
       <c r="C41" t="n" s="1">
         <v>44381.0</v>
@@ -1121,10 +1112,10 @@
     </row>
     <row r="42">
       <c r="A42" t="s">
+        <v>82</v>
+      </c>
+      <c r="B42" t="s">
         <v>83</v>
-      </c>
-      <c r="B42" t="s">
-        <v>84</v>
       </c>
       <c r="C42" t="n" s="1">
         <v>44388.0</v>
@@ -1132,10 +1123,10 @@
     </row>
     <row r="43">
       <c r="A43" t="s">
+        <v>84</v>
+      </c>
+      <c r="B43" t="s">
         <v>85</v>
-      </c>
-      <c r="B43" t="s">
-        <v>86</v>
       </c>
       <c r="C43" t="n" s="1">
         <v>44395.0</v>
@@ -1143,10 +1134,10 @@
     </row>
     <row r="44">
       <c r="A44" t="s">
+        <v>86</v>
+      </c>
+      <c r="B44" t="s">
         <v>87</v>
-      </c>
-      <c r="B44" t="s">
-        <v>88</v>
       </c>
       <c r="C44" t="n" s="1">
         <v>44402.0</v>
@@ -1154,10 +1145,10 @@
     </row>
     <row r="45">
       <c r="A45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B45" t="s">
         <v>89</v>
-      </c>
-      <c r="B45" t="s">
-        <v>90</v>
       </c>
       <c r="C45" t="n" s="1">
         <v>44409.0</v>
@@ -1165,10 +1156,10 @@
     </row>
     <row r="46">
       <c r="A46" t="s">
+        <v>90</v>
+      </c>
+      <c r="B46" t="s">
         <v>91</v>
-      </c>
-      <c r="B46" t="s">
-        <v>92</v>
       </c>
       <c r="C46" t="n" s="1">
         <v>44416.0</v>
@@ -1176,10 +1167,10 @@
     </row>
     <row r="47">
       <c r="A47" t="s">
+        <v>92</v>
+      </c>
+      <c r="B47" t="s">
         <v>93</v>
-      </c>
-      <c r="B47" t="s">
-        <v>94</v>
       </c>
       <c r="C47" t="n" s="1">
         <v>44423.0</v>
@@ -1187,10 +1178,10 @@
     </row>
     <row r="48">
       <c r="A48" t="s">
+        <v>94</v>
+      </c>
+      <c r="B48" t="s">
         <v>95</v>
-      </c>
-      <c r="B48" t="s">
-        <v>96</v>
       </c>
       <c r="C48" t="n" s="1">
         <v>44430.0</v>
@@ -1198,10 +1189,10 @@
     </row>
     <row r="49">
       <c r="A49" t="s">
+        <v>96</v>
+      </c>
+      <c r="B49" t="s">
         <v>97</v>
-      </c>
-      <c r="B49" t="s">
-        <v>98</v>
       </c>
       <c r="C49" t="n" s="1">
         <v>44437.0</v>
@@ -1209,10 +1200,10 @@
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B50" t="s">
-        <v>100</v>
+        <v>38</v>
       </c>
       <c r="C50" t="n" s="1">
         <v>44444.0</v>
@@ -1220,10 +1211,10 @@
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B51" t="s">
-        <v>44</v>
+        <v>100</v>
       </c>
       <c r="C51" t="n" s="1">
         <v>44451.0</v>
@@ -1231,10 +1222,10 @@
     </row>
     <row r="52">
       <c r="A52" t="s">
+        <v>101</v>
+      </c>
+      <c r="B52" t="s">
         <v>102</v>
-      </c>
-      <c r="B52" t="s">
-        <v>103</v>
       </c>
       <c r="C52" t="n" s="1">
         <v>44458.0</v>
@@ -1242,10 +1233,10 @@
     </row>
     <row r="53">
       <c r="A53" t="s">
+        <v>103</v>
+      </c>
+      <c r="B53" t="s">
         <v>104</v>
-      </c>
-      <c r="B53" t="s">
-        <v>105</v>
       </c>
       <c r="C53" t="n" s="1">
         <v>44465.0</v>
@@ -1253,10 +1244,10 @@
     </row>
     <row r="54">
       <c r="A54" t="s">
+        <v>105</v>
+      </c>
+      <c r="B54" t="s">
         <v>106</v>
-      </c>
-      <c r="B54" t="s">
-        <v>107</v>
       </c>
       <c r="C54" t="n" s="1">
         <v>44472.0</v>
@@ -1264,10 +1255,10 @@
     </row>
     <row r="55">
       <c r="A55" t="s">
+        <v>107</v>
+      </c>
+      <c r="B55" t="s">
         <v>108</v>
-      </c>
-      <c r="B55" t="s">
-        <v>109</v>
       </c>
       <c r="C55" t="n" s="1">
         <v>44479.041666666664</v>
@@ -1275,10 +1266,10 @@
     </row>
     <row r="56">
       <c r="A56" t="s">
+        <v>109</v>
+      </c>
+      <c r="B56" t="s">
         <v>110</v>
-      </c>
-      <c r="B56" t="s">
-        <v>111</v>
       </c>
       <c r="C56" t="n" s="1">
         <v>44486.041666666664</v>
@@ -1286,10 +1277,10 @@
     </row>
     <row r="57">
       <c r="A57" t="s">
+        <v>111</v>
+      </c>
+      <c r="B57" t="s">
         <v>112</v>
-      </c>
-      <c r="B57" t="s">
-        <v>113</v>
       </c>
       <c r="C57" t="n" s="1">
         <v>44493.041666666664</v>
@@ -1297,10 +1288,10 @@
     </row>
     <row r="58">
       <c r="A58" t="s">
+        <v>113</v>
+      </c>
+      <c r="B58" t="s">
         <v>114</v>
-      </c>
-      <c r="B58" t="s">
-        <v>115</v>
       </c>
       <c r="C58" t="n" s="1">
         <v>44500.041666666664</v>
@@ -1308,10 +1299,10 @@
     </row>
     <row r="59">
       <c r="A59" t="s">
+        <v>115</v>
+      </c>
+      <c r="B59" t="s">
         <v>116</v>
-      </c>
-      <c r="B59" t="s">
-        <v>117</v>
       </c>
       <c r="C59" t="n" s="1">
         <v>44507.041666666664</v>
@@ -1319,10 +1310,10 @@
     </row>
     <row r="60">
       <c r="A60" t="s">
+        <v>117</v>
+      </c>
+      <c r="B60" t="s">
         <v>118</v>
-      </c>
-      <c r="B60" t="s">
-        <v>72</v>
       </c>
       <c r="C60" t="n" s="1">
         <v>44514.041666666664</v>
@@ -1517,10 +1508,10 @@
     </row>
     <row r="78">
       <c r="A78" t="s">
+        <v>25</v>
+      </c>
+      <c r="B78" t="s">
         <v>153</v>
-      </c>
-      <c r="B78" t="s">
-        <v>154</v>
       </c>
       <c r="C78" t="n" s="1">
         <v>44640.041666666664</v>
@@ -1528,10 +1519,10 @@
     </row>
     <row r="79">
       <c r="A79" t="s">
+        <v>154</v>
+      </c>
+      <c r="B79" t="s">
         <v>155</v>
-      </c>
-      <c r="B79" t="s">
-        <v>156</v>
       </c>
       <c r="C79" t="n" s="1">
         <v>44647.041666666664</v>
@@ -1539,10 +1530,10 @@
     </row>
     <row r="80">
       <c r="A80" t="s">
+        <v>156</v>
+      </c>
+      <c r="B80" t="s">
         <v>157</v>
-      </c>
-      <c r="B80" t="s">
-        <v>158</v>
       </c>
       <c r="C80" t="n" s="1">
         <v>44654.041666666664</v>
@@ -1550,10 +1541,10 @@
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B81" t="s">
-        <v>160</v>
+        <v>60</v>
       </c>
       <c r="C81" t="n" s="1">
         <v>44661.0</v>
@@ -1561,10 +1552,10 @@
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B82" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C82" t="n" s="1">
         <v>44668.0</v>
@@ -1572,10 +1563,10 @@
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B83" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C83" t="n" s="1">
         <v>44675.0</v>
@@ -1583,10 +1574,10 @@
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B84" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C84" t="n" s="1">
         <v>44682.0</v>
@@ -1594,10 +1585,10 @@
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B85" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C85" t="n" s="1">
         <v>44689.0</v>
@@ -1605,10 +1596,10 @@
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B86" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C86" t="n" s="1">
         <v>44696.0</v>
@@ -1616,10 +1607,10 @@
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B87" t="s">
-        <v>172</v>
+        <v>28</v>
       </c>
       <c r="C87" t="n" s="1">
         <v>44703.0</v>
@@ -1627,10 +1618,10 @@
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B88" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C88" t="n" s="1">
         <v>44710.0</v>
@@ -1638,10 +1629,10 @@
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B89" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C89" t="n" s="1">
         <v>44717.0</v>
@@ -1649,10 +1640,10 @@
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B90" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C90" t="n" s="1">
         <v>44724.0</v>
@@ -1660,10 +1651,10 @@
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B91" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C91" t="n" s="1">
         <v>44731.0</v>
@@ -1671,10 +1662,10 @@
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B92" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C92" t="n" s="1">
         <v>44738.0</v>
@@ -1682,10 +1673,10 @@
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B93" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C93" t="n" s="1">
         <v>44745.0</v>
@@ -1693,10 +1684,10 @@
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B94" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C94" t="n" s="1">
         <v>44752.0</v>
@@ -1704,10 +1695,10 @@
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B95" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C95" t="n" s="1">
         <v>44759.0</v>
@@ -1715,10 +1706,10 @@
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B96" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C96" t="n" s="1">
         <v>44766.0</v>
@@ -1726,10 +1717,10 @@
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B97" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C97" t="n" s="1">
         <v>44773.0</v>
@@ -1737,10 +1728,10 @@
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B98" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C98" t="n" s="1">
         <v>44780.0</v>
@@ -1748,10 +1739,10 @@
     </row>
     <row r="99">
       <c r="A99" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B99" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C99" t="n" s="1">
         <v>44787.0</v>
@@ -1759,10 +1750,10 @@
     </row>
     <row r="100">
       <c r="A100" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B100" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C100" t="n" s="1">
         <v>44794.0</v>
@@ -1770,10 +1761,10 @@
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B101" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C101" t="n" s="1">
         <v>44801.0</v>

</xml_diff>

<commit_message>
Add a couple of lines to the readme and add a test for a simple sheet using the fluent style
</commit_message>
<xml_diff>
--- a/output/fluentmanyrows.xlsx
+++ b/output/fluentmanyrows.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="202">
   <si>
     <t>Name</t>
   </si>
@@ -23,598 +23,601 @@
     <t>Hired</t>
   </si>
   <si>
-    <t>Alyce Auer</t>
-  </si>
-  <si>
-    <t>Regional Design Associate</t>
-  </si>
-  <si>
-    <t>Young Shields</t>
-  </si>
-  <si>
-    <t>International Administration Engineer</t>
-  </si>
-  <si>
-    <t>Ms. Florence Bechtelar</t>
-  </si>
-  <si>
-    <t>Future Design Coordinator</t>
-  </si>
-  <si>
-    <t>Mayme Witting III</t>
-  </si>
-  <si>
-    <t>District Advertising Agent</t>
-  </si>
-  <si>
-    <t>Ms. Federico Crona</t>
-  </si>
-  <si>
-    <t>Healthcare Orchestrator</t>
-  </si>
-  <si>
-    <t>Lorette Altenwerth</t>
-  </si>
-  <si>
-    <t>Future Community-Services Executive</t>
-  </si>
-  <si>
-    <t>Haywood Stiedemann</t>
-  </si>
-  <si>
-    <t>Legal Consultant</t>
-  </si>
-  <si>
-    <t>Joana Cummerata</t>
-  </si>
-  <si>
-    <t>Future Banking Supervisor</t>
-  </si>
-  <si>
-    <t>Ms. Ricky Glover</t>
-  </si>
-  <si>
-    <t>Mining Specialist</t>
-  </si>
-  <si>
-    <t>Martin Adams</t>
-  </si>
-  <si>
-    <t>Internal Farming Associate</t>
-  </si>
-  <si>
-    <t>Forrest Bailey V</t>
-  </si>
-  <si>
-    <t>Hospitality Strategist</t>
-  </si>
-  <si>
-    <t>Latasha Feeney</t>
-  </si>
-  <si>
-    <t>Future Administration Planner</t>
-  </si>
-  <si>
-    <t>Anastasia Jacobs PhD</t>
-  </si>
-  <si>
-    <t>Product Marketing Analyst</t>
-  </si>
-  <si>
-    <t>Lashell Stracke</t>
-  </si>
-  <si>
-    <t>Hospitality Technician</t>
-  </si>
-  <si>
-    <t>Quinn Gleichner V</t>
-  </si>
-  <si>
-    <t>Global Consulting Architect</t>
-  </si>
-  <si>
-    <t>Pierre Osinski PhD</t>
-  </si>
-  <si>
-    <t>Principal Community-Services Consultant</t>
-  </si>
-  <si>
-    <t>Armando Lind DDS</t>
-  </si>
-  <si>
-    <t>National Community-Services Architect</t>
-  </si>
-  <si>
-    <t>Thad Schaden</t>
-  </si>
-  <si>
-    <t>Dynamic Banking Strategist</t>
-  </si>
-  <si>
-    <t>Coy Moore</t>
-  </si>
-  <si>
-    <t>Technology Coordinator</t>
-  </si>
-  <si>
-    <t>Ms. Damion D'Amore</t>
-  </si>
-  <si>
-    <t>Marketing Coordinator</t>
-  </si>
-  <si>
-    <t>Benjamin Cremin</t>
-  </si>
-  <si>
-    <t>Central Real-Estate Manager</t>
-  </si>
-  <si>
-    <t>Mrs. Hershel Wiza</t>
-  </si>
-  <si>
-    <t>Raymon Lebsack</t>
-  </si>
-  <si>
-    <t>Hospitality Manager</t>
-  </si>
-  <si>
-    <t>Mellisa Rolfson</t>
-  </si>
-  <si>
-    <t>Education Coordinator</t>
-  </si>
-  <si>
-    <t>Brandie Kris</t>
-  </si>
-  <si>
-    <t>Consulting Supervisor</t>
-  </si>
-  <si>
-    <t>Loma Schowalter Sr.</t>
-  </si>
-  <si>
-    <t>Mining Orchestrator</t>
-  </si>
-  <si>
-    <t>Mr. Adolph Kulas</t>
-  </si>
-  <si>
-    <t>Retail Agent</t>
-  </si>
-  <si>
-    <t>Mrs. Mauricio D'Amore</t>
-  </si>
-  <si>
-    <t>Hospitality Officer</t>
-  </si>
-  <si>
-    <t>Lewis Smith</t>
-  </si>
-  <si>
-    <t>Customer Education Architect</t>
-  </si>
-  <si>
-    <t>Terrence Rutherford</t>
-  </si>
-  <si>
-    <t>National Legal Manager</t>
-  </si>
-  <si>
-    <t>Gretchen Blick</t>
-  </si>
-  <si>
-    <t>Lead Government Architect</t>
-  </si>
-  <si>
-    <t>Peter Schowalter II</t>
-  </si>
-  <si>
-    <t>Lead Sales Supervisor</t>
-  </si>
-  <si>
-    <t>Wally Gorczany</t>
-  </si>
-  <si>
-    <t>IT Designer</t>
-  </si>
-  <si>
-    <t>Lanny Collins</t>
-  </si>
-  <si>
-    <t>Global Advertising Specialist</t>
-  </si>
-  <si>
-    <t>Mrs. Bertram Wilderman</t>
-  </si>
-  <si>
-    <t>Global Manager</t>
-  </si>
-  <si>
-    <t>Michel O'Conner</t>
-  </si>
-  <si>
-    <t>National Government Coordinator</t>
-  </si>
-  <si>
-    <t>Clemente Ankunding MD</t>
-  </si>
-  <si>
-    <t>Banking Orchestrator</t>
-  </si>
-  <si>
-    <t>Tisa Lueilwitz</t>
+    <t>Rey Nikolaus</t>
+  </si>
+  <si>
+    <t>Legacy Supervisor</t>
+  </si>
+  <si>
+    <t>Shandi Kuhic</t>
+  </si>
+  <si>
+    <t>Human Planner</t>
+  </si>
+  <si>
+    <t>Ty Hettinger PhD</t>
+  </si>
+  <si>
+    <t>Advertising Manager</t>
+  </si>
+  <si>
+    <t>Salvador Schumm</t>
+  </si>
+  <si>
+    <t>Accounting Officer</t>
+  </si>
+  <si>
+    <t>Rick Hessel</t>
+  </si>
+  <si>
+    <t>Advertising Director</t>
+  </si>
+  <si>
+    <t>Romana Blanda</t>
+  </si>
+  <si>
+    <t>Dynamic Banking Specialist</t>
+  </si>
+  <si>
+    <t>Mitch Fisher</t>
+  </si>
+  <si>
+    <t>Technology Liaison</t>
+  </si>
+  <si>
+    <t>Amada Runte</t>
+  </si>
+  <si>
+    <t>Mining Technician</t>
+  </si>
+  <si>
+    <t>Mckinley Toy II</t>
+  </si>
+  <si>
+    <t>Human Community-Services Specialist</t>
+  </si>
+  <si>
+    <t>Margarett Watsica II</t>
+  </si>
+  <si>
+    <t>IT Developer</t>
+  </si>
+  <si>
+    <t>Ouida Gulgowski</t>
+  </si>
+  <si>
+    <t>Senior Technology Supervisor</t>
+  </si>
+  <si>
+    <t>Mr. Jame Macejkovic</t>
+  </si>
+  <si>
+    <t>Lead Representative</t>
+  </si>
+  <si>
+    <t>Marty Jast</t>
+  </si>
+  <si>
+    <t>Internal Retail Administrator</t>
+  </si>
+  <si>
+    <t>Yer Carroll</t>
+  </si>
+  <si>
+    <t>International Director</t>
+  </si>
+  <si>
+    <t>Reginald Roberts</t>
+  </si>
+  <si>
+    <t>Principal Hospitality Coordinator</t>
+  </si>
+  <si>
+    <t>Emil Christiansen</t>
+  </si>
+  <si>
+    <t>IT Assistant</t>
+  </si>
+  <si>
+    <t>Bennie Nolan DVM</t>
+  </si>
+  <si>
+    <t>Accounting Associate</t>
+  </si>
+  <si>
+    <t>Rigoberto Boyer IV</t>
+  </si>
+  <si>
+    <t>Sales Director</t>
+  </si>
+  <si>
+    <t>Cherryl Glover</t>
+  </si>
+  <si>
+    <t>Future Healthcare Liaison</t>
+  </si>
+  <si>
+    <t>Merissa Tremblay</t>
+  </si>
+  <si>
+    <t>Legal Planner</t>
+  </si>
+  <si>
+    <t>Frank Hahn V</t>
+  </si>
+  <si>
+    <t>District Producer</t>
+  </si>
+  <si>
+    <t>Jasper Bernier MD</t>
+  </si>
+  <si>
+    <t>District Manufacturing Representative</t>
+  </si>
+  <si>
+    <t>Marguerite Rempel</t>
+  </si>
+  <si>
+    <t>Product Community-Services Associate</t>
+  </si>
+  <si>
+    <t>Miss Loida Goodwin</t>
+  </si>
+  <si>
+    <t>Senior Healthcare Facilitator</t>
+  </si>
+  <si>
+    <t>Tessa O'Keefe</t>
+  </si>
+  <si>
+    <t>Chief Facilitator</t>
+  </si>
+  <si>
+    <t>Olen Buckridge</t>
+  </si>
+  <si>
+    <t>National Education Designer</t>
+  </si>
+  <si>
+    <t>Oren Corwin</t>
+  </si>
+  <si>
+    <t>Advertising Representative</t>
+  </si>
+  <si>
+    <t>Jasmin Predovic</t>
+  </si>
+  <si>
+    <t>District Director</t>
+  </si>
+  <si>
+    <t>Mrs. Marlin Farrell</t>
+  </si>
+  <si>
+    <t>Regional Representative</t>
+  </si>
+  <si>
+    <t>Keven Mitchell</t>
+  </si>
+  <si>
+    <t>Human Technology Representative</t>
+  </si>
+  <si>
+    <t>Hosea Volkman</t>
+  </si>
+  <si>
+    <t>Administration Strategist</t>
+  </si>
+  <si>
+    <t>Daniel Ankunding</t>
+  </si>
+  <si>
+    <t>Marketing Producer</t>
+  </si>
+  <si>
+    <t>Angle Cormier</t>
+  </si>
+  <si>
+    <t>Future Hospitality Coordinator</t>
+  </si>
+  <si>
+    <t>Issac King</t>
+  </si>
+  <si>
+    <t>Internal IT Officer</t>
+  </si>
+  <si>
+    <t>Darius Kutch I</t>
+  </si>
+  <si>
+    <t>Legacy Farming Strategist</t>
+  </si>
+  <si>
+    <t>Wendell Feil</t>
+  </si>
+  <si>
+    <t>National Retail Facilitator</t>
+  </si>
+  <si>
+    <t>Scotty Effertz</t>
+  </si>
+  <si>
+    <t>International Sales Executive</t>
+  </si>
+  <si>
+    <t>Floyd Okuneva</t>
+  </si>
+  <si>
+    <t>Education Technician</t>
+  </si>
+  <si>
+    <t>Becki Christiansen</t>
+  </si>
+  <si>
+    <t>Senior Technology Administrator</t>
+  </si>
+  <si>
+    <t>Fausto Kihn I</t>
+  </si>
+  <si>
+    <t>Investor Strategist</t>
+  </si>
+  <si>
+    <t>Mrs. Adrienne McClure</t>
+  </si>
+  <si>
+    <t>Lead IT Supervisor</t>
+  </si>
+  <si>
+    <t>Keith Pfeffer</t>
+  </si>
+  <si>
+    <t>Customer Administrator</t>
+  </si>
+  <si>
+    <t>Rodolfo Jenkins</t>
+  </si>
+  <si>
+    <t>Retail Officer</t>
+  </si>
+  <si>
+    <t>Mrs. Vance Rohan</t>
+  </si>
+  <si>
+    <t>Chief Farming Engineer</t>
+  </si>
+  <si>
+    <t>Olivia Kutch IV</t>
+  </si>
+  <si>
+    <t>International Marketing Supervisor</t>
+  </si>
+  <si>
+    <t>Hosea Flatley</t>
+  </si>
+  <si>
+    <t>Administration Specialist</t>
+  </si>
+  <si>
+    <t>Hyman O'Kon</t>
+  </si>
+  <si>
+    <t>Senior Administration Technician</t>
+  </si>
+  <si>
+    <t>Miss Buena Kertzmann</t>
+  </si>
+  <si>
+    <t>Alfonso Hegmann</t>
   </si>
   <si>
     <t>Farming Planner</t>
   </si>
   <si>
-    <t>Mrs. Moises Witting</t>
-  </si>
-  <si>
-    <t>Hospitality Liaison</t>
-  </si>
-  <si>
-    <t>Teddy Swift</t>
-  </si>
-  <si>
-    <t>Global Community-Services Analyst</t>
-  </si>
-  <si>
-    <t>Lucila Schumm Jr.</t>
-  </si>
-  <si>
-    <t>Sales Analyst</t>
-  </si>
-  <si>
-    <t>Johnny Bins</t>
-  </si>
-  <si>
-    <t>Central Architect</t>
-  </si>
-  <si>
-    <t>Elton Collins</t>
-  </si>
-  <si>
-    <t>Forward Manufacturing Director</t>
-  </si>
-  <si>
-    <t>Jackson Corkery</t>
-  </si>
-  <si>
-    <t>Investor Manufacturing Coordinator</t>
-  </si>
-  <si>
-    <t>Kelsie Kuphal</t>
-  </si>
-  <si>
-    <t>Manufacturing Coordinator</t>
-  </si>
-  <si>
-    <t>Mr. Garfield Tillman</t>
-  </si>
-  <si>
-    <t>International Real-Estate Specialist</t>
-  </si>
-  <si>
-    <t>Estella Spencer</t>
-  </si>
-  <si>
-    <t>Chief Manager</t>
-  </si>
-  <si>
-    <t>Camilla Kunze III</t>
-  </si>
-  <si>
-    <t>Marketing Associate</t>
-  </si>
-  <si>
-    <t>Cody Haag</t>
-  </si>
-  <si>
-    <t>Global Design Consultant</t>
-  </si>
-  <si>
-    <t>Lynn Upton</t>
-  </si>
-  <si>
-    <t>Advertising Engineer</t>
-  </si>
-  <si>
-    <t>Adrianna Cummerata</t>
-  </si>
-  <si>
-    <t>Technology Technician</t>
-  </si>
-  <si>
-    <t>Brain Satterfield</t>
-  </si>
-  <si>
-    <t>Farming Officer</t>
-  </si>
-  <si>
-    <t>Ariel Johnson</t>
-  </si>
-  <si>
-    <t>National Designer</t>
-  </si>
-  <si>
-    <t>Mickey Cassin</t>
-  </si>
-  <si>
-    <t>Administration Representative</t>
-  </si>
-  <si>
-    <t>Jonathon Powlowski</t>
-  </si>
-  <si>
-    <t>International Advertising Representative</t>
-  </si>
-  <si>
-    <t>Ms. Elna Bode</t>
-  </si>
-  <si>
-    <t>Chief Construction Analyst</t>
-  </si>
-  <si>
-    <t>Emil Kreiger MD</t>
-  </si>
-  <si>
-    <t>Marketing Executive</t>
-  </si>
-  <si>
-    <t>Allyson Kuhic</t>
-  </si>
-  <si>
-    <t>Corporate Marketing Orchestrator</t>
-  </si>
-  <si>
-    <t>Kacie Grimes V</t>
-  </si>
-  <si>
-    <t>Corporate Healthcare Planner</t>
-  </si>
-  <si>
-    <t>Miss Hilario Bode</t>
-  </si>
-  <si>
-    <t>Corporate Administration Engineer</t>
-  </si>
-  <si>
-    <t>Miss Cecilia Feest</t>
-  </si>
-  <si>
-    <t>Global Construction Assistant</t>
-  </si>
-  <si>
-    <t>Ernestine Zboncak</t>
-  </si>
-  <si>
-    <t>Corporate Design Executive</t>
-  </si>
-  <si>
-    <t>Carmelia Heaney</t>
-  </si>
-  <si>
-    <t>Global Design Developer</t>
-  </si>
-  <si>
-    <t>Raven Friesen</t>
-  </si>
-  <si>
-    <t>Direct Farming Liaison</t>
-  </si>
-  <si>
-    <t>Saul Kuhic</t>
-  </si>
-  <si>
-    <t>Sales Facilitator</t>
-  </si>
-  <si>
-    <t>Toney Schamberger</t>
-  </si>
-  <si>
-    <t>Human Construction Engineer</t>
-  </si>
-  <si>
-    <t>Virgina Schimmel MD</t>
-  </si>
-  <si>
-    <t>National Hospitality Strategist</t>
-  </si>
-  <si>
-    <t>Ms. Daphine Skiles</t>
-  </si>
-  <si>
-    <t>Government Strategist</t>
-  </si>
-  <si>
-    <t>Bebe Rogahn</t>
-  </si>
-  <si>
-    <t>Future Mining Liaison</t>
-  </si>
-  <si>
-    <t>Valentin Reichert</t>
-  </si>
-  <si>
-    <t>Lead Advertising Executive</t>
-  </si>
-  <si>
-    <t>Cheryle Nader DDS</t>
-  </si>
-  <si>
-    <t>Hospitality Executive</t>
-  </si>
-  <si>
-    <t>Napoleon Corkery</t>
-  </si>
-  <si>
-    <t>Central Legal Strategist</t>
-  </si>
-  <si>
-    <t>Fairy Nolan</t>
-  </si>
-  <si>
-    <t>Global Analyst</t>
-  </si>
-  <si>
-    <t>Hortense Prosacco</t>
-  </si>
-  <si>
-    <t>Administration Officer</t>
-  </si>
-  <si>
-    <t>Ingeborg Wisozk Sr.</t>
-  </si>
-  <si>
-    <t>Hospitality Architect</t>
-  </si>
-  <si>
-    <t>Debbi Beer</t>
-  </si>
-  <si>
-    <t>Legacy Farming Administrator</t>
-  </si>
-  <si>
-    <t>Marya Feest</t>
-  </si>
-  <si>
-    <t>Regional Construction Facilitator</t>
-  </si>
-  <si>
-    <t>Classie Feeney</t>
-  </si>
-  <si>
-    <t>Technology Facilitator</t>
-  </si>
-  <si>
-    <t>Jody McKenzie</t>
-  </si>
-  <si>
-    <t>Senior IT Director</t>
-  </si>
-  <si>
-    <t>Bibi Kirlin</t>
-  </si>
-  <si>
-    <t>Farming Executive</t>
-  </si>
-  <si>
-    <t>Branda Boyer</t>
-  </si>
-  <si>
-    <t>Product Community-Services Officer</t>
-  </si>
-  <si>
-    <t>Wilbur Hauck</t>
-  </si>
-  <si>
-    <t>Internal Manufacturing Supervisor</t>
-  </si>
-  <si>
-    <t>Dillon Berge</t>
-  </si>
-  <si>
-    <t>Forward Executive</t>
-  </si>
-  <si>
-    <t>Rory Von</t>
-  </si>
-  <si>
-    <t>Global IT Planner</t>
-  </si>
-  <si>
-    <t>Joey O'Kon</t>
-  </si>
-  <si>
-    <t>Eldon Effertz</t>
-  </si>
-  <si>
-    <t>Direct Strategist</t>
-  </si>
-  <si>
-    <t>Corie Larson PhD</t>
-  </si>
-  <si>
-    <t>Direct Construction Developer</t>
-  </si>
-  <si>
-    <t>Blaine Langworth MD</t>
-  </si>
-  <si>
-    <t>Sales Associate</t>
-  </si>
-  <si>
-    <t>Miss Lyda Kuvalis</t>
-  </si>
-  <si>
-    <t>Investor Consulting Consultant</t>
-  </si>
-  <si>
-    <t>Kurtis Von</t>
-  </si>
-  <si>
-    <t>National Government Designer</t>
-  </si>
-  <si>
-    <t>Ms. Lory Swift</t>
-  </si>
-  <si>
-    <t>Real-Estate Executive</t>
-  </si>
-  <si>
-    <t>Jamel Nolan</t>
-  </si>
-  <si>
-    <t>Human Hospitality Director</t>
-  </si>
-  <si>
-    <t>Dr. Stacey McDermott</t>
-  </si>
-  <si>
-    <t>Central IT Agent</t>
-  </si>
-  <si>
-    <t>Mrs. Lamonica Grimes</t>
-  </si>
-  <si>
-    <t>Customer Manager</t>
-  </si>
-  <si>
-    <t>Cliff Schmeler</t>
-  </si>
-  <si>
-    <t>Human Administrator</t>
-  </si>
-  <si>
-    <t>Emmanuel Emmerich</t>
-  </si>
-  <si>
-    <t>Customer Design Supervisor</t>
-  </si>
-  <si>
-    <t>Ressie Weimann</t>
-  </si>
-  <si>
-    <t>Manufacturing Director</t>
-  </si>
-  <si>
-    <t>Jeni Olson</t>
-  </si>
-  <si>
-    <t>Corporate Executive</t>
-  </si>
-  <si>
-    <t>Gerry McCullough MD</t>
-  </si>
-  <si>
-    <t>Real-Estate Manager</t>
-  </si>
-  <si>
-    <t>Shera Morar</t>
-  </si>
-  <si>
-    <t>Retail Representative</t>
+    <t>Alphonse Quigley MD</t>
+  </si>
+  <si>
+    <t>Corporate Marketing Representative</t>
+  </si>
+  <si>
+    <t>Ferdinand Cormier</t>
+  </si>
+  <si>
+    <t>Lead IT Associate</t>
+  </si>
+  <si>
+    <t>Lynna Macejkovic</t>
+  </si>
+  <si>
+    <t>Legacy Technician</t>
+  </si>
+  <si>
+    <t>Loree Lueilwitz</t>
+  </si>
+  <si>
+    <t>Community-Services Consultant</t>
+  </si>
+  <si>
+    <t>Eric McCullough</t>
+  </si>
+  <si>
+    <t>Human Mining Coordinator</t>
+  </si>
+  <si>
+    <t>Deloise Maggio</t>
+  </si>
+  <si>
+    <t>Investor IT Agent</t>
+  </si>
+  <si>
+    <t>Otilia Haag</t>
+  </si>
+  <si>
+    <t>Marketing Analyst</t>
+  </si>
+  <si>
+    <t>Duncan Anderson</t>
+  </si>
+  <si>
+    <t>Forward Design Representative</t>
+  </si>
+  <si>
+    <t>Kelly Franecki</t>
+  </si>
+  <si>
+    <t>Global Technician</t>
+  </si>
+  <si>
+    <t>Mr. Orval Sipes</t>
+  </si>
+  <si>
+    <t>Customer Technician</t>
+  </si>
+  <si>
+    <t>Brent Dibbert V</t>
+  </si>
+  <si>
+    <t>Human Marketing Orchestrator</t>
+  </si>
+  <si>
+    <t>Shirley Jerde</t>
+  </si>
+  <si>
+    <t>Direct Accounting Consultant</t>
+  </si>
+  <si>
+    <t>Antonetta Goyette</t>
+  </si>
+  <si>
+    <t>Investor Retail Coordinator</t>
+  </si>
+  <si>
+    <t>Miss Salvador Kovacek</t>
+  </si>
+  <si>
+    <t>Future Government Analyst</t>
+  </si>
+  <si>
+    <t>Miss Cornelius Little</t>
+  </si>
+  <si>
+    <t>Corporate Healthcare Architect</t>
+  </si>
+  <si>
+    <t>Raul Armstrong</t>
+  </si>
+  <si>
+    <t>Manufacturing Liaison</t>
+  </si>
+  <si>
+    <t>Bailey Hoppe</t>
+  </si>
+  <si>
+    <t>Technology Representative</t>
+  </si>
+  <si>
+    <t>Robbi Medhurst</t>
+  </si>
+  <si>
+    <t>Principal Representative</t>
+  </si>
+  <si>
+    <t>Darla Rempel</t>
+  </si>
+  <si>
+    <t>Technology Officer</t>
+  </si>
+  <si>
+    <t>Deana Spencer</t>
+  </si>
+  <si>
+    <t>Future Coordinator</t>
+  </si>
+  <si>
+    <t>Bethany Connelly</t>
+  </si>
+  <si>
+    <t>Retail Designer</t>
+  </si>
+  <si>
+    <t>Galina Schaefer</t>
+  </si>
+  <si>
+    <t>Forward Developer</t>
+  </si>
+  <si>
+    <t>Dr. Brooks Beier</t>
+  </si>
+  <si>
+    <t>Technology Assistant</t>
+  </si>
+  <si>
+    <t>Cherise Schaden</t>
+  </si>
+  <si>
+    <t>Corporate Facilitator</t>
+  </si>
+  <si>
+    <t>Xuan Carter</t>
+  </si>
+  <si>
+    <t>Chief Executive</t>
+  </si>
+  <si>
+    <t>Quinton Price</t>
+  </si>
+  <si>
+    <t>Technology Developer</t>
+  </si>
+  <si>
+    <t>Jacqulyn O'Keefe PhD</t>
+  </si>
+  <si>
+    <t>Manufacturing Engineer</t>
+  </si>
+  <si>
+    <t>Lizeth Simonis DDS</t>
+  </si>
+  <si>
+    <t>Legacy Specialist</t>
+  </si>
+  <si>
+    <t>Theo Jacobi</t>
+  </si>
+  <si>
+    <t>Regional IT Consultant</t>
+  </si>
+  <si>
+    <t>Carolann Raynor</t>
+  </si>
+  <si>
+    <t>Direct Farming Designer</t>
+  </si>
+  <si>
+    <t>Toby Upton</t>
+  </si>
+  <si>
+    <t>Forward Manufacturing Producer</t>
+  </si>
+  <si>
+    <t>Jackie O'Kon</t>
+  </si>
+  <si>
+    <t>Government Specialist</t>
+  </si>
+  <si>
+    <t>Alphonse Jacobi</t>
+  </si>
+  <si>
+    <t>Internal Administrator</t>
+  </si>
+  <si>
+    <t>Cher Schiller IV</t>
+  </si>
+  <si>
+    <t>Legacy Design Manager</t>
+  </si>
+  <si>
+    <t>Josefa Wisozk</t>
+  </si>
+  <si>
+    <t>Legal Architect</t>
+  </si>
+  <si>
+    <t>Monte Rohan</t>
+  </si>
+  <si>
+    <t>Internal Planner</t>
+  </si>
+  <si>
+    <t>Larae Dickinson</t>
+  </si>
+  <si>
+    <t>Chief Education Planner</t>
+  </si>
+  <si>
+    <t>Marc Conn</t>
+  </si>
+  <si>
+    <t>Product Real-Estate Executive</t>
+  </si>
+  <si>
+    <t>Margo O'Conner</t>
+  </si>
+  <si>
+    <t>Product Facilitator</t>
+  </si>
+  <si>
+    <t>Micah Legros</t>
+  </si>
+  <si>
+    <t>Future Facilitator</t>
+  </si>
+  <si>
+    <t>Cornell Sauer</t>
+  </si>
+  <si>
+    <t>Lead IT Technician</t>
+  </si>
+  <si>
+    <t>Marilyn Quitzon</t>
+  </si>
+  <si>
+    <t>Corporate Associate</t>
+  </si>
+  <si>
+    <t>Refugio Crist V</t>
+  </si>
+  <si>
+    <t>Investor Associate</t>
+  </si>
+  <si>
+    <t>Myesha Von</t>
+  </si>
+  <si>
+    <t>International Executive</t>
+  </si>
+  <si>
+    <t>Mrs. Rodney Heathcote</t>
+  </si>
+  <si>
+    <t>Design Coordinator</t>
+  </si>
+  <si>
+    <t>Lakenya Waelchi</t>
+  </si>
+  <si>
+    <t>Real-Estate Orchestrator</t>
+  </si>
+  <si>
+    <t>Percy Grant</t>
+  </si>
+  <si>
+    <t>Future Advertising Manager</t>
+  </si>
+  <si>
+    <t>Mr. Rosanne Lynch</t>
+  </si>
+  <si>
+    <t>Design Executive</t>
+  </si>
+  <si>
+    <t>Donnell Goyette</t>
+  </si>
+  <si>
+    <t>Education Administrator</t>
+  </si>
+  <si>
+    <t>Mrs. Camelia Ritchie</t>
+  </si>
+  <si>
+    <t>Central IT Strategist</t>
+  </si>
+  <si>
+    <t>Olen Barrows</t>
+  </si>
+  <si>
+    <t>Customer Marketing Administrator</t>
   </si>
 </sst>
 </file>
@@ -1032,7 +1035,7 @@
         <v>45</v>
       </c>
       <c r="B23" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="C23" t="n" s="25">
         <v>44255.041666666664</v>
@@ -1040,10 +1043,10 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B24" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C24" t="n" s="26">
         <v>44262.041666666664</v>
@@ -1051,10 +1054,10 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B25" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C25" t="n" s="27">
         <v>44269.041666666664</v>
@@ -1062,10 +1065,10 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B26" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C26" t="n" s="28">
         <v>44276.041666666664</v>
@@ -1073,10 +1076,10 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B27" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C27" t="n" s="29">
         <v>44283.041666666664</v>
@@ -1084,10 +1087,10 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B28" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C28" t="n" s="30">
         <v>44290.041666666664</v>
@@ -1095,10 +1098,10 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B29" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C29" t="n" s="31">
         <v>44297.0</v>
@@ -1106,10 +1109,10 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B30" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C30" t="n" s="32">
         <v>44304.0</v>
@@ -1117,10 +1120,10 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B31" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C31" t="n" s="33">
         <v>44311.0</v>
@@ -1128,10 +1131,10 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B32" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C32" t="n" s="34">
         <v>44318.0</v>
@@ -1139,10 +1142,10 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B33" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C33" t="n" s="35">
         <v>44325.0</v>
@@ -1150,10 +1153,10 @@
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B34" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C34" t="n" s="36">
         <v>44332.0</v>
@@ -1161,10 +1164,10 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B35" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C35" t="n" s="37">
         <v>44339.0</v>
@@ -1172,10 +1175,10 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B36" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C36" t="n" s="38">
         <v>44346.0</v>
@@ -1183,10 +1186,10 @@
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B37" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C37" t="n" s="39">
         <v>44353.0</v>
@@ -1194,10 +1197,10 @@
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B38" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C38" t="n" s="40">
         <v>44360.0</v>
@@ -1205,10 +1208,10 @@
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B39" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C39" t="n" s="41">
         <v>44367.0</v>
@@ -1216,10 +1219,10 @@
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B40" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C40" t="n" s="42">
         <v>44374.0</v>
@@ -1227,10 +1230,10 @@
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B41" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C41" t="n" s="43">
         <v>44381.0</v>
@@ -1238,10 +1241,10 @@
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B42" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C42" t="n" s="44">
         <v>44388.0</v>
@@ -1249,10 +1252,10 @@
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B43" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C43" t="n" s="45">
         <v>44395.0</v>
@@ -1260,10 +1263,10 @@
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B44" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C44" t="n" s="46">
         <v>44402.0</v>
@@ -1271,10 +1274,10 @@
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B45" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C45" t="n" s="47">
         <v>44409.0</v>
@@ -1282,10 +1285,10 @@
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B46" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C46" t="n" s="48">
         <v>44416.0</v>
@@ -1293,10 +1296,10 @@
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B47" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C47" t="n" s="49">
         <v>44423.0</v>
@@ -1304,10 +1307,10 @@
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B48" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C48" t="n" s="50">
         <v>44430.0</v>
@@ -1315,10 +1318,10 @@
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B49" t="s">
-        <v>97</v>
+        <v>44</v>
       </c>
       <c r="C49" t="n" s="51">
         <v>44437.0</v>
@@ -1725,7 +1728,7 @@
         <v>170</v>
       </c>
       <c r="B86" t="s">
-        <v>51</v>
+        <v>171</v>
       </c>
       <c r="C86" t="n" s="88">
         <v>44696.0</v>
@@ -1733,10 +1736,10 @@
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B87" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C87" t="n" s="89">
         <v>44703.0</v>
@@ -1744,10 +1747,10 @@
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B88" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C88" t="n" s="90">
         <v>44710.0</v>
@@ -1755,10 +1758,10 @@
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B89" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C89" t="n" s="91">
         <v>44717.0</v>
@@ -1766,10 +1769,10 @@
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B90" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C90" t="n" s="92">
         <v>44724.0</v>
@@ -1777,10 +1780,10 @@
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B91" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C91" t="n" s="93">
         <v>44731.0</v>
@@ -1788,10 +1791,10 @@
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B92" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C92" t="n" s="94">
         <v>44738.0</v>
@@ -1799,10 +1802,10 @@
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B93" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C93" t="n" s="95">
         <v>44745.0</v>
@@ -1810,10 +1813,10 @@
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B94" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C94" t="n" s="96">
         <v>44752.0</v>
@@ -1821,10 +1824,10 @@
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B95" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C95" t="n" s="97">
         <v>44759.0</v>
@@ -1832,10 +1835,10 @@
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B96" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C96" t="n" s="98">
         <v>44766.0</v>
@@ -1843,10 +1846,10 @@
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B97" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C97" t="n" s="99">
         <v>44773.0</v>
@@ -1854,10 +1857,10 @@
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B98" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C98" t="n" s="100">
         <v>44780.0</v>
@@ -1865,10 +1868,10 @@
     </row>
     <row r="99">
       <c r="A99" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B99" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C99" t="n" s="101">
         <v>44787.0</v>
@@ -1876,10 +1879,10 @@
     </row>
     <row r="100">
       <c r="A100" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B100" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C100" t="n" s="102">
         <v>44794.0</v>
@@ -1887,10 +1890,10 @@
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B101" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C101" t="n" s="103">
         <v>44801.0</v>

</xml_diff>

<commit_message>
add an erase() method to the Sheet
</commit_message>
<xml_diff>
--- a/output/fluentmanyrows.xlsx
+++ b/output/fluentmanyrows.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="203">
   <si>
     <t>Name</t>
   </si>
@@ -23,589 +23,604 @@
     <t>Hired</t>
   </si>
   <si>
-    <t>Ezra Thiel</t>
-  </si>
-  <si>
-    <t>Chief Advertising Engineer</t>
-  </si>
-  <si>
-    <t>Amiee Goldner</t>
-  </si>
-  <si>
-    <t>Marketing Liaison</t>
-  </si>
-  <si>
-    <t>Elena Abernathy</t>
-  </si>
-  <si>
-    <t>Customer Mining Producer</t>
-  </si>
-  <si>
-    <t>Catrice Daniel</t>
-  </si>
-  <si>
-    <t>Education Director</t>
-  </si>
-  <si>
-    <t>Delbert Torphy</t>
-  </si>
-  <si>
-    <t>Design Strategist</t>
-  </si>
-  <si>
-    <t>Romona Schneider</t>
-  </si>
-  <si>
-    <t>Global Consulting Analyst</t>
-  </si>
-  <si>
-    <t>Elida Collier</t>
-  </si>
-  <si>
-    <t>International Construction Facilitator</t>
-  </si>
-  <si>
-    <t>Spring Hermiston</t>
-  </si>
-  <si>
-    <t>Farming Architect</t>
-  </si>
-  <si>
-    <t>Mrs. Ngoc Larkin</t>
-  </si>
-  <si>
-    <t>Investor Administration Assistant</t>
-  </si>
-  <si>
-    <t>Mrs. Lonny Schaefer</t>
-  </si>
-  <si>
-    <t>Hospitality Officer</t>
-  </si>
-  <si>
-    <t>Leonore Kiehn</t>
-  </si>
-  <si>
-    <t>Banking Facilitator</t>
-  </si>
-  <si>
-    <t>Abe Weissnat</t>
-  </si>
-  <si>
-    <t>Regional Real-Estate Administrator</t>
-  </si>
-  <si>
-    <t>Susanne Sporer</t>
-  </si>
-  <si>
-    <t>Real-Estate Liaison</t>
-  </si>
-  <si>
-    <t>Susanne Medhurst</t>
-  </si>
-  <si>
-    <t>Construction Designer</t>
-  </si>
-  <si>
-    <t>Bea Schuster</t>
-  </si>
-  <si>
-    <t>IT Representative</t>
-  </si>
-  <si>
-    <t>Starr Koepp II</t>
-  </si>
-  <si>
-    <t>Forward Marketing Planner</t>
-  </si>
-  <si>
-    <t>Davina Greenfelder V</t>
-  </si>
-  <si>
-    <t>Central Accounting Associate</t>
-  </si>
-  <si>
-    <t>Rachael Lang Sr.</t>
-  </si>
-  <si>
-    <t>Dynamic Developer</t>
-  </si>
-  <si>
-    <t>Bari Veum</t>
-  </si>
-  <si>
-    <t>Hospitality Producer</t>
-  </si>
-  <si>
-    <t>Agripina Rogahn</t>
-  </si>
-  <si>
-    <t>Direct Retail Consultant</t>
-  </si>
-  <si>
-    <t>Matthew Jerde</t>
-  </si>
-  <si>
-    <t>Internal Engineer</t>
-  </si>
-  <si>
-    <t>Miss Jeremiah Murazik</t>
-  </si>
-  <si>
-    <t>District Banking Representative</t>
-  </si>
-  <si>
-    <t>Santo Ankunding</t>
-  </si>
-  <si>
-    <t>Principal Accounting Agent</t>
-  </si>
-  <si>
-    <t>Miss Karry Balistreri</t>
-  </si>
-  <si>
-    <t>Sales Analyst</t>
-  </si>
-  <si>
-    <t>Elroy Skiles DVM</t>
-  </si>
-  <si>
-    <t>Product Agent</t>
-  </si>
-  <si>
-    <t>Chrissy Stanton</t>
-  </si>
-  <si>
-    <t>Future Sales Consultant</t>
-  </si>
-  <si>
-    <t>Kris Connelly</t>
-  </si>
-  <si>
-    <t>Product Hospitality Director</t>
-  </si>
-  <si>
-    <t>Mr. Owen Lang</t>
-  </si>
-  <si>
-    <t>Lead Community-Services Officer</t>
-  </si>
-  <si>
-    <t>Minh Medhurst</t>
-  </si>
-  <si>
-    <t>Central Designer</t>
-  </si>
-  <si>
-    <t>Orlando Hettinger V</t>
-  </si>
-  <si>
-    <t>Marketing Associate</t>
-  </si>
-  <si>
-    <t>Dr. Bernardina Ebert</t>
-  </si>
-  <si>
-    <t>Design Assistant</t>
-  </si>
-  <si>
-    <t>Joanie MacGyver II</t>
-  </si>
-  <si>
-    <t>Healthcare Specialist</t>
-  </si>
-  <si>
-    <t>Miss Jeromy Osinski</t>
-  </si>
-  <si>
-    <t>Marketing Director</t>
-  </si>
-  <si>
-    <t>Adalberto Hyatt</t>
-  </si>
-  <si>
-    <t>Direct Government Liaison</t>
-  </si>
-  <si>
-    <t>Wilfred Kohler</t>
-  </si>
-  <si>
-    <t>Consulting Administrator</t>
-  </si>
-  <si>
-    <t>Tinisha Casper DVM</t>
-  </si>
-  <si>
-    <t>Farming Assistant</t>
-  </si>
-  <si>
-    <t>Jillian Gorczany</t>
-  </si>
-  <si>
-    <t>Product Manufacturing Architect</t>
-  </si>
-  <si>
-    <t>Irene Cole</t>
-  </si>
-  <si>
-    <t>Human Farming Officer</t>
-  </si>
-  <si>
-    <t>Madalyn Rath</t>
-  </si>
-  <si>
-    <t>Miss Latonia Satterfield</t>
-  </si>
-  <si>
-    <t>Chief Orchestrator</t>
-  </si>
-  <si>
-    <t>Jenine Rippin</t>
-  </si>
-  <si>
-    <t>Customer Hospitality Producer</t>
-  </si>
-  <si>
-    <t>Tyrell Becker</t>
-  </si>
-  <si>
-    <t>Manufacturing Agent</t>
-  </si>
-  <si>
-    <t>Dedra Douglas</t>
-  </si>
-  <si>
-    <t>Internal Construction Facilitator</t>
-  </si>
-  <si>
-    <t>Marion Langworth</t>
-  </si>
-  <si>
-    <t>International Associate</t>
-  </si>
-  <si>
-    <t>Genia Skiles</t>
-  </si>
-  <si>
-    <t>Retail Analyst</t>
-  </si>
-  <si>
-    <t>Cristina Koelpin MD</t>
-  </si>
-  <si>
-    <t>Hospitality Assistant</t>
-  </si>
-  <si>
-    <t>Jessika Schamberger</t>
-  </si>
-  <si>
-    <t>Investor Legal Producer</t>
-  </si>
-  <si>
-    <t>Miss Roxy Okuneva</t>
-  </si>
-  <si>
-    <t>Lead Producer</t>
-  </si>
-  <si>
-    <t>Gavin Mueller</t>
-  </si>
-  <si>
-    <t>Global Construction Strategist</t>
-  </si>
-  <si>
-    <t>Erwin Rempel Jr.</t>
-  </si>
-  <si>
-    <t>Human Mining Producer</t>
-  </si>
-  <si>
-    <t>Troy Christiansen</t>
-  </si>
-  <si>
-    <t>Principal Executive</t>
-  </si>
-  <si>
-    <t>Ross Jakubowski</t>
-  </si>
-  <si>
-    <t>Senior Mining Officer</t>
-  </si>
-  <si>
-    <t>Johnny Turcotte</t>
-  </si>
-  <si>
-    <t>District Technician</t>
-  </si>
-  <si>
-    <t>Lavona Kiehn</t>
-  </si>
-  <si>
-    <t>Direct Coordinator</t>
-  </si>
-  <si>
-    <t>Ms. Hector Hills</t>
-  </si>
-  <si>
-    <t>Central Agent</t>
-  </si>
-  <si>
-    <t>Quinton Paucek</t>
-  </si>
-  <si>
-    <t>Investor Mining Facilitator</t>
-  </si>
-  <si>
-    <t>Katheryn Hessel</t>
-  </si>
-  <si>
-    <t>National Consulting Planner</t>
-  </si>
-  <si>
-    <t>Leo Barton</t>
-  </si>
-  <si>
-    <t>Real-Estate Officer</t>
-  </si>
-  <si>
-    <t>Dr. Cristy Mante</t>
-  </si>
-  <si>
-    <t>Real-Estate Administrator</t>
-  </si>
-  <si>
-    <t>Wade Weimann</t>
-  </si>
-  <si>
-    <t>Central Strategist</t>
-  </si>
-  <si>
-    <t>Burton Cole</t>
-  </si>
-  <si>
-    <t>Mining Manager</t>
-  </si>
-  <si>
-    <t>Miss Sandy Kovacek</t>
-  </si>
-  <si>
-    <t>Barrett Steuber Jr.</t>
-  </si>
-  <si>
-    <t>Legal Supervisor</t>
-  </si>
-  <si>
-    <t>Sharita Wolf</t>
-  </si>
-  <si>
-    <t>Human Consulting Strategist</t>
-  </si>
-  <si>
-    <t>Nicky Okuneva V</t>
-  </si>
-  <si>
-    <t>Chief Director</t>
-  </si>
-  <si>
-    <t>Archie Hayes</t>
-  </si>
-  <si>
-    <t>Banking Technician</t>
-  </si>
-  <si>
-    <t>Stewart Blick PhD</t>
-  </si>
-  <si>
-    <t>Banking Planner</t>
-  </si>
-  <si>
-    <t>Dierdre O'Hara Sr.</t>
-  </si>
-  <si>
-    <t>Investor Community-Services Planner</t>
-  </si>
-  <si>
-    <t>Eve Kuhlman</t>
-  </si>
-  <si>
-    <t>Mining Director</t>
-  </si>
-  <si>
-    <t>Catherina O'Conner</t>
-  </si>
-  <si>
-    <t>Human Assistant</t>
-  </si>
-  <si>
-    <t>Guadalupe Krajcik</t>
-  </si>
-  <si>
-    <t>Corporate Engineer</t>
-  </si>
-  <si>
-    <t>Sol Lang</t>
-  </si>
-  <si>
-    <t>Future Consultant</t>
-  </si>
-  <si>
-    <t>Landon Pacocha</t>
-  </si>
-  <si>
-    <t>National Consulting Associate</t>
-  </si>
-  <si>
-    <t>Miss Kimberely Funk</t>
-  </si>
-  <si>
-    <t>Corporate Supervisor</t>
-  </si>
-  <si>
-    <t>Kendrick West III</t>
-  </si>
-  <si>
-    <t>Construction Director</t>
-  </si>
-  <si>
-    <t>Kara Feil</t>
-  </si>
-  <si>
-    <t>Principal Banking Consultant</t>
-  </si>
-  <si>
-    <t>Dr. Ramon Murazik</t>
+    <t>Darrel Dooley</t>
+  </si>
+  <si>
+    <t>Direct Associate</t>
+  </si>
+  <si>
+    <t>Miss Sulema Yost</t>
+  </si>
+  <si>
+    <t>District Legal Orchestrator</t>
+  </si>
+  <si>
+    <t>Aldo Oberbrunner</t>
+  </si>
+  <si>
+    <t>International Farming Liaison</t>
+  </si>
+  <si>
+    <t>Ms. Jeanine Hilll</t>
+  </si>
+  <si>
+    <t>Community-Services Administrator</t>
+  </si>
+  <si>
+    <t>Dr. Pete Bechtelar</t>
+  </si>
+  <si>
+    <t>Investor Director</t>
+  </si>
+  <si>
+    <t>Khadijah Boehm MD</t>
+  </si>
+  <si>
+    <t>Senior Administration Officer</t>
+  </si>
+  <si>
+    <t>Kurtis Murphy MD</t>
+  </si>
+  <si>
+    <t>District Orchestrator</t>
+  </si>
+  <si>
+    <t>Abigail Steuber</t>
+  </si>
+  <si>
+    <t>Consulting Specialist</t>
+  </si>
+  <si>
+    <t>Fawn Kshlerin</t>
+  </si>
+  <si>
+    <t>Direct Consulting Planner</t>
+  </si>
+  <si>
+    <t>Edwardo Price II</t>
+  </si>
+  <si>
+    <t>Customer IT Designer</t>
+  </si>
+  <si>
+    <t>Jeremiah Douglas</t>
+  </si>
+  <si>
+    <t>Government Executive</t>
+  </si>
+  <si>
+    <t>Carey Schmidt</t>
+  </si>
+  <si>
+    <t>Customer Mining Technician</t>
+  </si>
+  <si>
+    <t>Ms. Jeanice Schmeler</t>
+  </si>
+  <si>
+    <t>District Architect</t>
+  </si>
+  <si>
+    <t>Dottie Stiedemann</t>
+  </si>
+  <si>
+    <t>Government Designer</t>
+  </si>
+  <si>
+    <t>Pablo Hauck</t>
+  </si>
+  <si>
+    <t>Sales Developer</t>
+  </si>
+  <si>
+    <t>Davina Bernhard IV</t>
+  </si>
+  <si>
+    <t>Accounting Officer</t>
+  </si>
+  <si>
+    <t>Alfredia Bradtke</t>
+  </si>
+  <si>
+    <t>Senior Retail Architect</t>
+  </si>
+  <si>
+    <t>Trevor Runolfsson IV</t>
+  </si>
+  <si>
+    <t>Customer Mining Executive</t>
+  </si>
+  <si>
+    <t>Lon Mraz</t>
+  </si>
+  <si>
+    <t>Community-Services Associate</t>
+  </si>
+  <si>
+    <t>Dr. Ester Schmidt</t>
+  </si>
+  <si>
+    <t>Mining Orchestrator</t>
+  </si>
+  <si>
+    <t>Alphonse Ryan</t>
+  </si>
+  <si>
+    <t>Healthcare Agent</t>
+  </si>
+  <si>
+    <t>Donny Larson</t>
+  </si>
+  <si>
+    <t>Central Specialist</t>
+  </si>
+  <si>
+    <t>Myrl Gottlieb</t>
+  </si>
+  <si>
+    <t>Mining Developer</t>
+  </si>
+  <si>
+    <t>Earnest Rodriguez</t>
+  </si>
+  <si>
+    <t>Dynamic Design Engineer</t>
+  </si>
+  <si>
+    <t>Blondell Fritsch DDS</t>
+  </si>
+  <si>
+    <t>Global Technology Executive</t>
+  </si>
+  <si>
+    <t>Edwardo VonRueden</t>
+  </si>
+  <si>
+    <t>International Administration Assistant</t>
+  </si>
+  <si>
+    <t>Minerva Lindgren</t>
+  </si>
+  <si>
+    <t>IT Director</t>
+  </si>
+  <si>
+    <t>Kathie Torp</t>
+  </si>
+  <si>
+    <t>Dynamic Specialist</t>
+  </si>
+  <si>
+    <t>Toney Mertz</t>
+  </si>
+  <si>
+    <t>Legal Strategist</t>
+  </si>
+  <si>
+    <t>Janis Leannon Jr.</t>
+  </si>
+  <si>
+    <t>Community-Services Facilitator</t>
+  </si>
+  <si>
+    <t>Ezra Rodriguez</t>
+  </si>
+  <si>
+    <t>Senior IT Liaison</t>
+  </si>
+  <si>
+    <t>Israel Turcotte</t>
+  </si>
+  <si>
+    <t>Sales Liaison</t>
+  </si>
+  <si>
+    <t>Sulema Kris</t>
+  </si>
+  <si>
+    <t>Mining Strategist</t>
+  </si>
+  <si>
+    <t>Shon Frami</t>
+  </si>
+  <si>
+    <t>Central Assistant</t>
+  </si>
+  <si>
+    <t>Darwin Jones</t>
+  </si>
+  <si>
+    <t>Central Government Representative</t>
+  </si>
+  <si>
+    <t>Orval Upton</t>
+  </si>
+  <si>
+    <t>District Design Analyst</t>
+  </si>
+  <si>
+    <t>Ladonna Steuber</t>
+  </si>
+  <si>
+    <t>International Consulting Officer</t>
+  </si>
+  <si>
+    <t>Oliver Walker</t>
+  </si>
+  <si>
+    <t>Education Specialist</t>
+  </si>
+  <si>
+    <t>Troy O'Hara</t>
   </si>
   <si>
     <t>International Agent</t>
   </si>
   <si>
-    <t>Nicky Carroll</t>
-  </si>
-  <si>
-    <t>Global Government Technician</t>
-  </si>
-  <si>
-    <t>Michel Boyle</t>
-  </si>
-  <si>
-    <t>National Real-Estate Director</t>
-  </si>
-  <si>
-    <t>Mr. Arcelia Schuppe</t>
-  </si>
-  <si>
-    <t>Marketing Administrator</t>
-  </si>
-  <si>
-    <t>Dr. Junko Beier</t>
-  </si>
-  <si>
-    <t>Farming Associate</t>
-  </si>
-  <si>
-    <t>Evan Bernhard</t>
-  </si>
-  <si>
-    <t>National Accounting Producer</t>
-  </si>
-  <si>
-    <t>Wiley Dach</t>
-  </si>
-  <si>
-    <t>Vivan Quigley</t>
-  </si>
-  <si>
-    <t>Corporate Technology Facilitator</t>
-  </si>
-  <si>
-    <t>Anastacia Veum</t>
-  </si>
-  <si>
-    <t>Technology Facilitator</t>
-  </si>
-  <si>
-    <t>Randolph Schaefer</t>
-  </si>
-  <si>
-    <t>Regional Manufacturing Facilitator</t>
-  </si>
-  <si>
-    <t>Lita Aufderhar</t>
-  </si>
-  <si>
-    <t>District Hospitality Assistant</t>
-  </si>
-  <si>
-    <t>Miss Hassan Rutherford</t>
-  </si>
-  <si>
-    <t>Human Manufacturing Facilitator</t>
-  </si>
-  <si>
-    <t>Ashanti Crona PhD</t>
-  </si>
-  <si>
-    <t>Lead Administration Technician</t>
-  </si>
-  <si>
-    <t>Cari Bergstrom</t>
-  </si>
-  <si>
-    <t>National Technology Administrator</t>
-  </si>
-  <si>
-    <t>Ward Littel</t>
-  </si>
-  <si>
-    <t>Community-Services Specialist</t>
-  </si>
-  <si>
-    <t>Wilfred Zulauf</t>
-  </si>
-  <si>
-    <t>Ms. Erik Dibbert</t>
-  </si>
-  <si>
-    <t>Advertising Designer</t>
-  </si>
-  <si>
-    <t>Mrs. Jerrod Howell</t>
-  </si>
-  <si>
-    <t>Regional Healthcare Consultant</t>
-  </si>
-  <si>
-    <t>Louann Mueller</t>
-  </si>
-  <si>
-    <t>Design Planner</t>
-  </si>
-  <si>
-    <t>Darnell Lowe</t>
-  </si>
-  <si>
-    <t>National Design Supervisor</t>
-  </si>
-  <si>
-    <t>Griselda Jacobi</t>
-  </si>
-  <si>
-    <t>Principal Community-Services Producer</t>
-  </si>
-  <si>
-    <t>Curt Bogisich</t>
-  </si>
-  <si>
-    <t>Barbera Runolfsdottir</t>
-  </si>
-  <si>
-    <t>IT Associate</t>
-  </si>
-  <si>
-    <t>Shawn Cronin</t>
-  </si>
-  <si>
-    <t>Education Associate</t>
+    <t>Pandora Pagac</t>
+  </si>
+  <si>
+    <t>Senior Advertising Director</t>
+  </si>
+  <si>
+    <t>Velvet Weimann</t>
+  </si>
+  <si>
+    <t>Retail Producer</t>
+  </si>
+  <si>
+    <t>Ms. Brett Reinger</t>
+  </si>
+  <si>
+    <t>Principal Facilitator</t>
+  </si>
+  <si>
+    <t>Pasty Bosco</t>
+  </si>
+  <si>
+    <t>Mining Consultant</t>
+  </si>
+  <si>
+    <t>Latosha Ferry</t>
+  </si>
+  <si>
+    <t>Mining Designer</t>
+  </si>
+  <si>
+    <t>Zina Auer</t>
+  </si>
+  <si>
+    <t>Construction Executive</t>
+  </si>
+  <si>
+    <t>Mrs. Eusebia DuBuque</t>
+  </si>
+  <si>
+    <t>Education Representative</t>
+  </si>
+  <si>
+    <t>Freddie Stroman</t>
+  </si>
+  <si>
+    <t>Government Consultant</t>
+  </si>
+  <si>
+    <t>Jaye Klocko PhD</t>
+  </si>
+  <si>
+    <t>International Advertising Consultant</t>
+  </si>
+  <si>
+    <t>Miss Doloris Huels</t>
+  </si>
+  <si>
+    <t>Forward Legal Manager</t>
+  </si>
+  <si>
+    <t>Kirk Reichel</t>
+  </si>
+  <si>
+    <t>Banking Orchestrator</t>
+  </si>
+  <si>
+    <t>Adelaida Bins</t>
+  </si>
+  <si>
+    <t>Manufacturing Architect</t>
+  </si>
+  <si>
+    <t>Chantelle Hilpert</t>
+  </si>
+  <si>
+    <t>International Real-Estate Agent</t>
+  </si>
+  <si>
+    <t>Theron Hessel</t>
+  </si>
+  <si>
+    <t>Regional Mining Specialist</t>
+  </si>
+  <si>
+    <t>Mrs. Frederick Hartmann</t>
+  </si>
+  <si>
+    <t>Marketing Executive</t>
+  </si>
+  <si>
+    <t>Emery Mosciski</t>
+  </si>
+  <si>
+    <t>Legacy Construction Agent</t>
+  </si>
+  <si>
+    <t>Lashaunda Mayer</t>
+  </si>
+  <si>
+    <t>Human Hospitality Developer</t>
+  </si>
+  <si>
+    <t>Retta Reilly</t>
+  </si>
+  <si>
+    <t>Forward Assistant</t>
+  </si>
+  <si>
+    <t>Hosea Glover MD</t>
+  </si>
+  <si>
+    <t>International Officer</t>
+  </si>
+  <si>
+    <t>Guillermo Wilderman</t>
+  </si>
+  <si>
+    <t>Legacy Sales Consultant</t>
+  </si>
+  <si>
+    <t>Mr. Lennie Rippin</t>
+  </si>
+  <si>
+    <t>National Legal Director</t>
+  </si>
+  <si>
+    <t>Mac Frami</t>
+  </si>
+  <si>
+    <t>Chief Technician</t>
+  </si>
+  <si>
+    <t>Harland Schowalter</t>
+  </si>
+  <si>
+    <t>Forward Manufacturing Producer</t>
+  </si>
+  <si>
+    <t>Stephnie Beer</t>
+  </si>
+  <si>
+    <t>Global Community-Services Architect</t>
+  </si>
+  <si>
+    <t>Mrs. Maria Kub</t>
+  </si>
+  <si>
+    <t>Direct Representative</t>
+  </si>
+  <si>
+    <t>Dr. Melvin Mraz</t>
+  </si>
+  <si>
+    <t>Global Executive</t>
+  </si>
+  <si>
+    <t>Shaquita Howell Jr.</t>
+  </si>
+  <si>
+    <t>Investor Consulting Developer</t>
+  </si>
+  <si>
+    <t>Moises Hyatt Sr.</t>
+  </si>
+  <si>
+    <t>Lead Design Technician</t>
+  </si>
+  <si>
+    <t>Diann O'Reilly</t>
+  </si>
+  <si>
+    <t>Principal Mining Designer</t>
+  </si>
+  <si>
+    <t>Verdell Leuschke</t>
+  </si>
+  <si>
+    <t>Advertising Administrator</t>
+  </si>
+  <si>
+    <t>Benny Turcotte</t>
+  </si>
+  <si>
+    <t>Investor Community-Services Supervisor</t>
+  </si>
+  <si>
+    <t>Lino Hagenes</t>
+  </si>
+  <si>
+    <t>Product Healthcare Designer</t>
+  </si>
+  <si>
+    <t>Rudy Brekke II</t>
+  </si>
+  <si>
+    <t>Legacy Agent</t>
+  </si>
+  <si>
+    <t>Mrs. Javier Sipes</t>
+  </si>
+  <si>
+    <t>Advertising Facilitator</t>
+  </si>
+  <si>
+    <t>Quincy Bechtelar IV</t>
+  </si>
+  <si>
+    <t>Global Government Consultant</t>
+  </si>
+  <si>
+    <t>Kelley Kovacek</t>
+  </si>
+  <si>
+    <t>Human Coordinator</t>
+  </si>
+  <si>
+    <t>Hershel Mohr</t>
+  </si>
+  <si>
+    <t>Investor Technology Administrator</t>
+  </si>
+  <si>
+    <t>Foster Brown</t>
+  </si>
+  <si>
+    <t>District Farming Technician</t>
+  </si>
+  <si>
+    <t>Sheena Yundt</t>
+  </si>
+  <si>
+    <t>Education Strategist</t>
+  </si>
+  <si>
+    <t>Miss Rosetta Blick</t>
+  </si>
+  <si>
+    <t>Hospitality Coordinator</t>
+  </si>
+  <si>
+    <t>Ardis Gutmann III</t>
+  </si>
+  <si>
+    <t>Dynamic Designer</t>
+  </si>
+  <si>
+    <t>Sunshine Daniel</t>
+  </si>
+  <si>
+    <t>Principal Hospitality Engineer</t>
+  </si>
+  <si>
+    <t>Ms. Phillis Crooks</t>
+  </si>
+  <si>
+    <t>District Design Representative</t>
+  </si>
+  <si>
+    <t>Tammara Goodwin</t>
+  </si>
+  <si>
+    <t>National Retail Analyst</t>
+  </si>
+  <si>
+    <t>Mr. Danna Feest</t>
+  </si>
+  <si>
+    <t>International Specialist</t>
+  </si>
+  <si>
+    <t>Jene Schimmel DDS</t>
+  </si>
+  <si>
+    <t>International Consulting Agent</t>
+  </si>
+  <si>
+    <t>Bethany Hartmann MD</t>
+  </si>
+  <si>
+    <t>Construction Developer</t>
+  </si>
+  <si>
+    <t>Stephnie Mills</t>
+  </si>
+  <si>
+    <t>Government Associate</t>
+  </si>
+  <si>
+    <t>Dr. Robt Kuvalis</t>
+  </si>
+  <si>
+    <t>Farming Analyst</t>
+  </si>
+  <si>
+    <t>Irvin Roob</t>
+  </si>
+  <si>
+    <t>Legacy Sales Planner</t>
+  </si>
+  <si>
+    <t>Blythe Dare</t>
+  </si>
+  <si>
+    <t>National Legal Supervisor</t>
+  </si>
+  <si>
+    <t>Mrs. Rudolph Dach</t>
+  </si>
+  <si>
+    <t>Human Real-Estate Architect</t>
+  </si>
+  <si>
+    <t>Dr. Pearlie Feil</t>
+  </si>
+  <si>
+    <t>District Developer</t>
+  </si>
+  <si>
+    <t>Andrea Pagac</t>
+  </si>
+  <si>
+    <t>Dynamic Consulting Executive</t>
+  </si>
+  <si>
+    <t>Dr. Melida Herzog</t>
+  </si>
+  <si>
+    <t>Hospitality Planner</t>
+  </si>
+  <si>
+    <t>Roger Heaney</t>
+  </si>
+  <si>
+    <t>Advertising Orchestrator</t>
+  </si>
+  <si>
+    <t>Ms. Echo Hand</t>
+  </si>
+  <si>
+    <t>Real-Estate Specialist</t>
+  </si>
+  <si>
+    <t>Lucas Casper</t>
+  </si>
+  <si>
+    <t>Education Administrator</t>
+  </si>
+  <si>
+    <t>Royce Homenick V</t>
+  </si>
+  <si>
+    <t>Design Associate</t>
+  </si>
+  <si>
+    <t>Virgen Renner</t>
+  </si>
+  <si>
+    <t>Dynamic Representative</t>
+  </si>
+  <si>
+    <t>Mr. Chong Dicki</t>
+  </si>
+  <si>
+    <t>Community-Services Executive</t>
   </si>
 </sst>
 </file>
@@ -664,11 +679,6 @@
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
-  <cols>
-    <col min="1" max="1" width="22.15625" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="36.15234375" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="12.2421875" customWidth="true" bestFit="true"/>
-  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="1">
@@ -1104,7 +1114,7 @@
         <v>79</v>
       </c>
       <c r="B40" t="s">
-        <v>24</v>
+        <v>80</v>
       </c>
       <c r="C40" t="n" s="2">
         <v>44374.0</v>
@@ -1112,10 +1122,10 @@
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B41" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C41" t="n" s="2">
         <v>44381.0</v>
@@ -1123,10 +1133,10 @@
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B42" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C42" t="n" s="2">
         <v>44388.0</v>
@@ -1134,10 +1144,10 @@
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B43" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C43" t="n" s="2">
         <v>44395.0</v>
@@ -1145,10 +1155,10 @@
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B44" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C44" t="n" s="2">
         <v>44402.0</v>
@@ -1156,10 +1166,10 @@
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B45" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C45" t="n" s="2">
         <v>44409.0</v>
@@ -1167,10 +1177,10 @@
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B46" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C46" t="n" s="2">
         <v>44416.0</v>
@@ -1178,10 +1188,10 @@
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B47" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C47" t="n" s="2">
         <v>44423.0</v>
@@ -1189,10 +1199,10 @@
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B48" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C48" t="n" s="2">
         <v>44430.0</v>
@@ -1200,10 +1210,10 @@
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B49" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C49" t="n" s="2">
         <v>44437.0</v>
@@ -1211,10 +1221,10 @@
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B50" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C50" t="n" s="2">
         <v>44444.0</v>
@@ -1222,10 +1232,10 @@
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B51" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C51" t="n" s="2">
         <v>44451.0</v>
@@ -1233,10 +1243,10 @@
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B52" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C52" t="n" s="2">
         <v>44458.0</v>
@@ -1244,10 +1254,10 @@
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B53" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C53" t="n" s="2">
         <v>44465.0</v>
@@ -1255,10 +1265,10 @@
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B54" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C54" t="n" s="2">
         <v>44472.0</v>
@@ -1266,10 +1276,10 @@
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B55" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C55" t="n" s="2">
         <v>44479.041666666664</v>
@@ -1277,10 +1287,10 @@
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B56" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C56" t="n" s="2">
         <v>44486.041666666664</v>
@@ -1288,10 +1298,10 @@
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B57" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C57" t="n" s="2">
         <v>44493.041666666664</v>
@@ -1299,10 +1309,10 @@
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B58" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C58" t="n" s="2">
         <v>44500.041666666664</v>
@@ -1310,10 +1320,10 @@
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B59" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C59" t="n" s="2">
         <v>44507.041666666664</v>
@@ -1321,10 +1331,10 @@
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B60" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C60" t="n" s="2">
         <v>44514.041666666664</v>
@@ -1332,10 +1342,10 @@
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B61" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C61" t="n" s="2">
         <v>44521.041666666664</v>
@@ -1343,10 +1353,10 @@
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B62" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C62" t="n" s="2">
         <v>44528.041666666664</v>
@@ -1354,10 +1364,10 @@
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B63" t="s">
-        <v>72</v>
+        <v>126</v>
       </c>
       <c r="C63" t="n" s="2">
         <v>44535.041666666664</v>
@@ -1365,10 +1375,10 @@
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B64" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C64" t="n" s="2">
         <v>44542.041666666664</v>
@@ -1376,10 +1386,10 @@
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B65" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C65" t="n" s="2">
         <v>44549.041666666664</v>
@@ -1387,10 +1397,10 @@
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B66" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C66" t="n" s="2">
         <v>44556.041666666664</v>
@@ -1398,10 +1408,10 @@
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B67" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C67" t="n" s="2">
         <v>44563.041666666664</v>
@@ -1409,10 +1419,10 @@
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B68" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C68" t="n" s="2">
         <v>44570.041666666664</v>
@@ -1420,10 +1430,10 @@
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B69" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C69" t="n" s="2">
         <v>44577.041666666664</v>
@@ -1431,10 +1441,10 @@
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B70" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C70" t="n" s="2">
         <v>44584.041666666664</v>
@@ -1442,10 +1452,10 @@
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B71" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C71" t="n" s="2">
         <v>44591.041666666664</v>
@@ -1453,10 +1463,10 @@
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B72" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C72" t="n" s="2">
         <v>44598.041666666664</v>
@@ -1464,10 +1474,10 @@
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B73" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C73" t="n" s="2">
         <v>44605.041666666664</v>
@@ -1475,10 +1485,10 @@
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B74" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C74" t="n" s="2">
         <v>44612.041666666664</v>
@@ -1486,10 +1496,10 @@
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B75" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C75" t="n" s="2">
         <v>44619.041666666664</v>
@@ -1497,10 +1507,10 @@
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B76" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C76" t="n" s="2">
         <v>44626.041666666664</v>
@@ -1508,10 +1518,10 @@
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B77" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C77" t="n" s="2">
         <v>44633.041666666664</v>
@@ -1519,10 +1529,10 @@
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B78" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C78" t="n" s="2">
         <v>44640.041666666664</v>
@@ -1530,10 +1540,10 @@
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B79" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C79" t="n" s="2">
         <v>44647.041666666664</v>
@@ -1541,10 +1551,10 @@
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B80" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C80" t="n" s="2">
         <v>44654.041666666664</v>
@@ -1552,10 +1562,10 @@
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B81" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C81" t="n" s="2">
         <v>44661.0</v>
@@ -1563,10 +1573,10 @@
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B82" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C82" t="n" s="2">
         <v>44668.0</v>
@@ -1574,10 +1584,10 @@
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B83" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C83" t="n" s="2">
         <v>44675.0</v>
@@ -1585,10 +1595,10 @@
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B84" t="s">
-        <v>22</v>
+        <v>168</v>
       </c>
       <c r="C84" t="n" s="2">
         <v>44682.0</v>
@@ -1596,10 +1606,10 @@
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="B85" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="C85" t="n" s="2">
         <v>44689.0</v>
@@ -1607,10 +1617,10 @@
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B86" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="C86" t="n" s="2">
         <v>44696.0</v>
@@ -1618,10 +1628,10 @@
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="B87" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="C87" t="n" s="2">
         <v>44703.0</v>
@@ -1629,10 +1639,10 @@
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="B88" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="C88" t="n" s="2">
         <v>44710.0</v>
@@ -1640,10 +1650,10 @@
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="B89" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="C89" t="n" s="2">
         <v>44717.0</v>
@@ -1651,10 +1661,10 @@
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="B90" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="C90" t="n" s="2">
         <v>44724.0</v>
@@ -1662,10 +1672,10 @@
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="B91" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="C91" t="n" s="2">
         <v>44731.0</v>
@@ -1673,10 +1683,10 @@
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="B92" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="C92" t="n" s="2">
         <v>44738.0</v>
@@ -1684,10 +1694,10 @@
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="B93" t="s">
-        <v>160</v>
+        <v>186</v>
       </c>
       <c r="C93" t="n" s="2">
         <v>44745.0</v>
@@ -1695,10 +1705,10 @@
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="B94" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="C94" t="n" s="2">
         <v>44752.0</v>
@@ -1706,10 +1716,10 @@
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="B95" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="C95" t="n" s="2">
         <v>44759.0</v>
@@ -1717,10 +1727,10 @@
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="B96" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="C96" t="n" s="2">
         <v>44766.0</v>
@@ -1728,10 +1738,10 @@
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="B97" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="C97" t="n" s="2">
         <v>44773.0</v>
@@ -1739,10 +1749,10 @@
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="B98" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="C98" t="n" s="2">
         <v>44780.0</v>
@@ -1750,10 +1760,10 @@
     </row>
     <row r="99">
       <c r="A99" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="B99" t="s">
-        <v>50</v>
+        <v>198</v>
       </c>
       <c r="C99" t="n" s="2">
         <v>44787.0</v>
@@ -1761,10 +1771,10 @@
     </row>
     <row r="100">
       <c r="A100" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="B100" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="C100" t="n" s="2">
         <v>44794.0</v>
@@ -1772,10 +1782,10 @@
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="B101" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="C101" t="n" s="2">
         <v>44801.0</v>

</xml_diff>

<commit_message>
add Book specific exceptions
</commit_message>
<xml_diff>
--- a/output/fluentmanyrows.xlsx
+++ b/output/fluentmanyrows.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="201">
   <si>
     <t>Name</t>
   </si>
@@ -23,604 +23,598 @@
     <t>Hired</t>
   </si>
   <si>
-    <t>Darrel Dooley</t>
-  </si>
-  <si>
-    <t>Direct Associate</t>
-  </si>
-  <si>
-    <t>Miss Sulema Yost</t>
-  </si>
-  <si>
-    <t>District Legal Orchestrator</t>
-  </si>
-  <si>
-    <t>Aldo Oberbrunner</t>
-  </si>
-  <si>
-    <t>International Farming Liaison</t>
-  </si>
-  <si>
-    <t>Ms. Jeanine Hilll</t>
-  </si>
-  <si>
-    <t>Community-Services Administrator</t>
-  </si>
-  <si>
-    <t>Dr. Pete Bechtelar</t>
-  </si>
-  <si>
-    <t>Investor Director</t>
-  </si>
-  <si>
-    <t>Khadijah Boehm MD</t>
-  </si>
-  <si>
-    <t>Senior Administration Officer</t>
-  </si>
-  <si>
-    <t>Kurtis Murphy MD</t>
-  </si>
-  <si>
-    <t>District Orchestrator</t>
-  </si>
-  <si>
-    <t>Abigail Steuber</t>
-  </si>
-  <si>
-    <t>Consulting Specialist</t>
-  </si>
-  <si>
-    <t>Fawn Kshlerin</t>
-  </si>
-  <si>
-    <t>Direct Consulting Planner</t>
-  </si>
-  <si>
-    <t>Edwardo Price II</t>
-  </si>
-  <si>
-    <t>Customer IT Designer</t>
-  </si>
-  <si>
-    <t>Jeremiah Douglas</t>
-  </si>
-  <si>
-    <t>Government Executive</t>
-  </si>
-  <si>
-    <t>Carey Schmidt</t>
+    <t>Miss Bert Quitzon</t>
+  </si>
+  <si>
+    <t>Retail Producer</t>
+  </si>
+  <si>
+    <t>Grace Stamm</t>
+  </si>
+  <si>
+    <t>Investor Real-Estate Specialist</t>
+  </si>
+  <si>
+    <t>Arnoldo Schumm III</t>
+  </si>
+  <si>
+    <t>Internal Consulting Architect</t>
+  </si>
+  <si>
+    <t>Hiram Swift</t>
+  </si>
+  <si>
+    <t>Consulting Assistant</t>
+  </si>
+  <si>
+    <t>Gwen McLaughlin I</t>
+  </si>
+  <si>
+    <t>Accounting Representative</t>
+  </si>
+  <si>
+    <t>Felice Weimann</t>
+  </si>
+  <si>
+    <t>National Liaison</t>
+  </si>
+  <si>
+    <t>Nannie Hamill</t>
+  </si>
+  <si>
+    <t>Legacy Retail Orchestrator</t>
+  </si>
+  <si>
+    <t>Ms. Burt Osinski</t>
+  </si>
+  <si>
+    <t>Regional Real-Estate Agent</t>
+  </si>
+  <si>
+    <t>Sang Friesen</t>
+  </si>
+  <si>
+    <t>Education Analyst</t>
+  </si>
+  <si>
+    <t>Dr. Elvin Kunze</t>
+  </si>
+  <si>
+    <t>Human Education Analyst</t>
+  </si>
+  <si>
+    <t>Malcolm Buckridge</t>
+  </si>
+  <si>
+    <t>Customer Consulting Supervisor</t>
+  </si>
+  <si>
+    <t>Louise Kihn</t>
+  </si>
+  <si>
+    <t>National Farming Manager</t>
+  </si>
+  <si>
+    <t>Miss Louella Parker</t>
+  </si>
+  <si>
+    <t>Hospitality Engineer</t>
+  </si>
+  <si>
+    <t>Mr. Larissa Stroman</t>
+  </si>
+  <si>
+    <t>National Education Designer</t>
+  </si>
+  <si>
+    <t>Kris Kemmer</t>
+  </si>
+  <si>
+    <t>Consulting Facilitator</t>
+  </si>
+  <si>
+    <t>Ezra Goodwin</t>
+  </si>
+  <si>
+    <t>Investor Technology Supervisor</t>
+  </si>
+  <si>
+    <t>Garry Gulgowski</t>
+  </si>
+  <si>
+    <t>Government Orchestrator</t>
+  </si>
+  <si>
+    <t>Marybelle Trantow</t>
+  </si>
+  <si>
+    <t>Internal Real-Estate Administrator</t>
+  </si>
+  <si>
+    <t>Delma Beahan</t>
+  </si>
+  <si>
+    <t>Manufacturing Developer</t>
+  </si>
+  <si>
+    <t>Griselda Wolf</t>
+  </si>
+  <si>
+    <t>Global Officer</t>
+  </si>
+  <si>
+    <t>Kenna Schmitt</t>
+  </si>
+  <si>
+    <t>Product Associate</t>
+  </si>
+  <si>
+    <t>Wilber DuBuque</t>
+  </si>
+  <si>
+    <t>Product Education Specialist</t>
+  </si>
+  <si>
+    <t>Kam Bailey</t>
+  </si>
+  <si>
+    <t>Hospitality Associate</t>
+  </si>
+  <si>
+    <t>Jackson Walter</t>
+  </si>
+  <si>
+    <t>Design Analyst</t>
+  </si>
+  <si>
+    <t>Mrs. Reita Rowe</t>
+  </si>
+  <si>
+    <t>Advertising Assistant</t>
+  </si>
+  <si>
+    <t>Berta Quigley</t>
+  </si>
+  <si>
+    <t>Community-Services Supervisor</t>
+  </si>
+  <si>
+    <t>Cleveland Volkman</t>
+  </si>
+  <si>
+    <t>Design Coordinator</t>
+  </si>
+  <si>
+    <t>Ria Schowalter PhD</t>
+  </si>
+  <si>
+    <t>Forward Assistant</t>
+  </si>
+  <si>
+    <t>Annmarie Buckridge I</t>
+  </si>
+  <si>
+    <t>Legal Developer</t>
+  </si>
+  <si>
+    <t>Francisco Hettinger</t>
+  </si>
+  <si>
+    <t>Education Strategist</t>
+  </si>
+  <si>
+    <t>Louise Corwin V</t>
+  </si>
+  <si>
+    <t>Mining Analyst</t>
+  </si>
+  <si>
+    <t>Gavin Ward</t>
+  </si>
+  <si>
+    <t>Customer Marketing Developer</t>
+  </si>
+  <si>
+    <t>Denver Schroeder</t>
+  </si>
+  <si>
+    <t>Manufacturing Engineer</t>
+  </si>
+  <si>
+    <t>Lawerence Hoppe</t>
+  </si>
+  <si>
+    <t>Technology Architect</t>
+  </si>
+  <si>
+    <t>Lakeesha Jacobson</t>
+  </si>
+  <si>
+    <t>Direct Developer</t>
+  </si>
+  <si>
+    <t>Augustine O'Hara MD</t>
+  </si>
+  <si>
+    <t>Mining Specialist</t>
+  </si>
+  <si>
+    <t>Jacki Harvey III</t>
+  </si>
+  <si>
+    <t>Forward Developer</t>
+  </si>
+  <si>
+    <t>Tomika Kohler Jr.</t>
+  </si>
+  <si>
+    <t>Senior Consulting Orchestrator</t>
+  </si>
+  <si>
+    <t>Chung Bahringer DDS</t>
+  </si>
+  <si>
+    <t>Customer IT Specialist</t>
+  </si>
+  <si>
+    <t>Miss Tommie Fadel</t>
+  </si>
+  <si>
+    <t>Administration Specialist</t>
+  </si>
+  <si>
+    <t>Ezekiel Funk</t>
+  </si>
+  <si>
+    <t>Internal Accounting Strategist</t>
+  </si>
+  <si>
+    <t>Hilma Wolff</t>
   </si>
   <si>
     <t>Customer Mining Technician</t>
   </si>
   <si>
-    <t>Ms. Jeanice Schmeler</t>
-  </si>
-  <si>
-    <t>District Architect</t>
-  </si>
-  <si>
-    <t>Dottie Stiedemann</t>
-  </si>
-  <si>
-    <t>Government Designer</t>
-  </si>
-  <si>
-    <t>Pablo Hauck</t>
-  </si>
-  <si>
-    <t>Sales Developer</t>
-  </si>
-  <si>
-    <t>Davina Bernhard IV</t>
-  </si>
-  <si>
-    <t>Accounting Officer</t>
-  </si>
-  <si>
-    <t>Alfredia Bradtke</t>
-  </si>
-  <si>
-    <t>Senior Retail Architect</t>
-  </si>
-  <si>
-    <t>Trevor Runolfsson IV</t>
-  </si>
-  <si>
-    <t>Customer Mining Executive</t>
-  </si>
-  <si>
-    <t>Lon Mraz</t>
-  </si>
-  <si>
-    <t>Community-Services Associate</t>
-  </si>
-  <si>
-    <t>Dr. Ester Schmidt</t>
-  </si>
-  <si>
-    <t>Mining Orchestrator</t>
-  </si>
-  <si>
-    <t>Alphonse Ryan</t>
-  </si>
-  <si>
-    <t>Healthcare Agent</t>
-  </si>
-  <si>
-    <t>Donny Larson</t>
-  </si>
-  <si>
-    <t>Central Specialist</t>
-  </si>
-  <si>
-    <t>Myrl Gottlieb</t>
-  </si>
-  <si>
-    <t>Mining Developer</t>
-  </si>
-  <si>
-    <t>Earnest Rodriguez</t>
-  </si>
-  <si>
-    <t>Dynamic Design Engineer</t>
-  </si>
-  <si>
-    <t>Blondell Fritsch DDS</t>
-  </si>
-  <si>
-    <t>Global Technology Executive</t>
-  </si>
-  <si>
-    <t>Edwardo VonRueden</t>
-  </si>
-  <si>
-    <t>International Administration Assistant</t>
-  </si>
-  <si>
-    <t>Minerva Lindgren</t>
-  </si>
-  <si>
-    <t>IT Director</t>
-  </si>
-  <si>
-    <t>Kathie Torp</t>
-  </si>
-  <si>
-    <t>Dynamic Specialist</t>
-  </si>
-  <si>
-    <t>Toney Mertz</t>
-  </si>
-  <si>
-    <t>Legal Strategist</t>
-  </si>
-  <si>
-    <t>Janis Leannon Jr.</t>
-  </si>
-  <si>
-    <t>Community-Services Facilitator</t>
-  </si>
-  <si>
-    <t>Ezra Rodriguez</t>
-  </si>
-  <si>
-    <t>Senior IT Liaison</t>
-  </si>
-  <si>
-    <t>Israel Turcotte</t>
-  </si>
-  <si>
-    <t>Sales Liaison</t>
-  </si>
-  <si>
-    <t>Sulema Kris</t>
-  </si>
-  <si>
-    <t>Mining Strategist</t>
-  </si>
-  <si>
-    <t>Shon Frami</t>
-  </si>
-  <si>
-    <t>Central Assistant</t>
-  </si>
-  <si>
-    <t>Darwin Jones</t>
-  </si>
-  <si>
-    <t>Central Government Representative</t>
-  </si>
-  <si>
-    <t>Orval Upton</t>
-  </si>
-  <si>
-    <t>District Design Analyst</t>
-  </si>
-  <si>
-    <t>Ladonna Steuber</t>
-  </si>
-  <si>
-    <t>International Consulting Officer</t>
-  </si>
-  <si>
-    <t>Oliver Walker</t>
-  </si>
-  <si>
-    <t>Education Specialist</t>
-  </si>
-  <si>
-    <t>Troy O'Hara</t>
-  </si>
-  <si>
-    <t>International Agent</t>
-  </si>
-  <si>
-    <t>Pandora Pagac</t>
-  </si>
-  <si>
-    <t>Senior Advertising Director</t>
-  </si>
-  <si>
-    <t>Velvet Weimann</t>
-  </si>
-  <si>
-    <t>Retail Producer</t>
-  </si>
-  <si>
-    <t>Ms. Brett Reinger</t>
-  </si>
-  <si>
-    <t>Principal Facilitator</t>
-  </si>
-  <si>
-    <t>Pasty Bosco</t>
-  </si>
-  <si>
-    <t>Mining Consultant</t>
-  </si>
-  <si>
-    <t>Latosha Ferry</t>
-  </si>
-  <si>
-    <t>Mining Designer</t>
-  </si>
-  <si>
-    <t>Zina Auer</t>
-  </si>
-  <si>
-    <t>Construction Executive</t>
-  </si>
-  <si>
-    <t>Mrs. Eusebia DuBuque</t>
-  </si>
-  <si>
-    <t>Education Representative</t>
-  </si>
-  <si>
-    <t>Freddie Stroman</t>
-  </si>
-  <si>
-    <t>Government Consultant</t>
-  </si>
-  <si>
-    <t>Jaye Klocko PhD</t>
-  </si>
-  <si>
-    <t>International Advertising Consultant</t>
-  </si>
-  <si>
-    <t>Miss Doloris Huels</t>
-  </si>
-  <si>
-    <t>Forward Legal Manager</t>
-  </si>
-  <si>
-    <t>Kirk Reichel</t>
-  </si>
-  <si>
-    <t>Banking Orchestrator</t>
-  </si>
-  <si>
-    <t>Adelaida Bins</t>
-  </si>
-  <si>
-    <t>Manufacturing Architect</t>
-  </si>
-  <si>
-    <t>Chantelle Hilpert</t>
-  </si>
-  <si>
-    <t>International Real-Estate Agent</t>
-  </si>
-  <si>
-    <t>Theron Hessel</t>
-  </si>
-  <si>
-    <t>Regional Mining Specialist</t>
-  </si>
-  <si>
-    <t>Mrs. Frederick Hartmann</t>
-  </si>
-  <si>
-    <t>Marketing Executive</t>
-  </si>
-  <si>
-    <t>Emery Mosciski</t>
-  </si>
-  <si>
-    <t>Legacy Construction Agent</t>
-  </si>
-  <si>
-    <t>Lashaunda Mayer</t>
-  </si>
-  <si>
-    <t>Human Hospitality Developer</t>
-  </si>
-  <si>
-    <t>Retta Reilly</t>
-  </si>
-  <si>
-    <t>Forward Assistant</t>
-  </si>
-  <si>
-    <t>Hosea Glover MD</t>
-  </si>
-  <si>
-    <t>International Officer</t>
-  </si>
-  <si>
-    <t>Guillermo Wilderman</t>
-  </si>
-  <si>
-    <t>Legacy Sales Consultant</t>
-  </si>
-  <si>
-    <t>Mr. Lennie Rippin</t>
-  </si>
-  <si>
-    <t>National Legal Director</t>
-  </si>
-  <si>
-    <t>Mac Frami</t>
-  </si>
-  <si>
-    <t>Chief Technician</t>
-  </si>
-  <si>
-    <t>Harland Schowalter</t>
-  </si>
-  <si>
-    <t>Forward Manufacturing Producer</t>
-  </si>
-  <si>
-    <t>Stephnie Beer</t>
-  </si>
-  <si>
-    <t>Global Community-Services Architect</t>
-  </si>
-  <si>
-    <t>Mrs. Maria Kub</t>
-  </si>
-  <si>
-    <t>Direct Representative</t>
-  </si>
-  <si>
-    <t>Dr. Melvin Mraz</t>
-  </si>
-  <si>
-    <t>Global Executive</t>
-  </si>
-  <si>
-    <t>Shaquita Howell Jr.</t>
-  </si>
-  <si>
-    <t>Investor Consulting Developer</t>
-  </si>
-  <si>
-    <t>Moises Hyatt Sr.</t>
-  </si>
-  <si>
-    <t>Lead Design Technician</t>
-  </si>
-  <si>
-    <t>Diann O'Reilly</t>
-  </si>
-  <si>
-    <t>Principal Mining Designer</t>
-  </si>
-  <si>
-    <t>Verdell Leuschke</t>
-  </si>
-  <si>
-    <t>Advertising Administrator</t>
-  </si>
-  <si>
-    <t>Benny Turcotte</t>
-  </si>
-  <si>
-    <t>Investor Community-Services Supervisor</t>
-  </si>
-  <si>
-    <t>Lino Hagenes</t>
-  </si>
-  <si>
-    <t>Product Healthcare Designer</t>
-  </si>
-  <si>
-    <t>Rudy Brekke II</t>
-  </si>
-  <si>
-    <t>Legacy Agent</t>
-  </si>
-  <si>
-    <t>Mrs. Javier Sipes</t>
-  </si>
-  <si>
-    <t>Advertising Facilitator</t>
-  </si>
-  <si>
-    <t>Quincy Bechtelar IV</t>
-  </si>
-  <si>
-    <t>Global Government Consultant</t>
-  </si>
-  <si>
-    <t>Kelley Kovacek</t>
-  </si>
-  <si>
-    <t>Human Coordinator</t>
-  </si>
-  <si>
-    <t>Hershel Mohr</t>
-  </si>
-  <si>
-    <t>Investor Technology Administrator</t>
-  </si>
-  <si>
-    <t>Foster Brown</t>
-  </si>
-  <si>
-    <t>District Farming Technician</t>
-  </si>
-  <si>
-    <t>Sheena Yundt</t>
-  </si>
-  <si>
-    <t>Education Strategist</t>
-  </si>
-  <si>
-    <t>Miss Rosetta Blick</t>
-  </si>
-  <si>
-    <t>Hospitality Coordinator</t>
-  </si>
-  <si>
-    <t>Ardis Gutmann III</t>
-  </si>
-  <si>
-    <t>Dynamic Designer</t>
-  </si>
-  <si>
-    <t>Sunshine Daniel</t>
-  </si>
-  <si>
-    <t>Principal Hospitality Engineer</t>
-  </si>
-  <si>
-    <t>Ms. Phillis Crooks</t>
-  </si>
-  <si>
-    <t>District Design Representative</t>
-  </si>
-  <si>
-    <t>Tammara Goodwin</t>
-  </si>
-  <si>
-    <t>National Retail Analyst</t>
-  </si>
-  <si>
-    <t>Mr. Danna Feest</t>
-  </si>
-  <si>
-    <t>International Specialist</t>
-  </si>
-  <si>
-    <t>Jene Schimmel DDS</t>
-  </si>
-  <si>
-    <t>International Consulting Agent</t>
-  </si>
-  <si>
-    <t>Bethany Hartmann MD</t>
-  </si>
-  <si>
-    <t>Construction Developer</t>
-  </si>
-  <si>
-    <t>Stephnie Mills</t>
-  </si>
-  <si>
-    <t>Government Associate</t>
-  </si>
-  <si>
-    <t>Dr. Robt Kuvalis</t>
+    <t>Stacy Medhurst IV</t>
+  </si>
+  <si>
+    <t>Corporate Administration Assistant</t>
+  </si>
+  <si>
+    <t>Miss Demarcus Schimmel</t>
+  </si>
+  <si>
+    <t>Hospitality Strategist</t>
+  </si>
+  <si>
+    <t>Jules Muller</t>
+  </si>
+  <si>
+    <t>Administration Representative</t>
+  </si>
+  <si>
+    <t>Mr. Michel Rath</t>
+  </si>
+  <si>
+    <t>Consulting Designer</t>
+  </si>
+  <si>
+    <t>Mrs. Maire Harber</t>
+  </si>
+  <si>
+    <t>Design Planner</t>
+  </si>
+  <si>
+    <t>Albertha Marvin</t>
+  </si>
+  <si>
+    <t>Healthcare Specialist</t>
+  </si>
+  <si>
+    <t>Mrs. Lawanna Glover</t>
+  </si>
+  <si>
+    <t>Investor Strategist</t>
+  </si>
+  <si>
+    <t>Steve Hessel</t>
+  </si>
+  <si>
+    <t>Corporate Government Analyst</t>
+  </si>
+  <si>
+    <t>Alejandro Gislason</t>
+  </si>
+  <si>
+    <t>Chief Coordinator</t>
+  </si>
+  <si>
+    <t>Carol Kshlerin IV</t>
+  </si>
+  <si>
+    <t>Chief Farming Technician</t>
+  </si>
+  <si>
+    <t>Pedro Bruen</t>
+  </si>
+  <si>
+    <t>Future Healthcare Orchestrator</t>
+  </si>
+  <si>
+    <t>Julian Christiansen III</t>
+  </si>
+  <si>
+    <t>Regional Administration Supervisor</t>
+  </si>
+  <si>
+    <t>Janina Rodriguez</t>
+  </si>
+  <si>
+    <t>Product Consulting Executive</t>
+  </si>
+  <si>
+    <t>Aretha Zulauf I</t>
+  </si>
+  <si>
+    <t>Legal Producer</t>
+  </si>
+  <si>
+    <t>Dr. Evonne Thompson</t>
   </si>
   <si>
     <t>Farming Analyst</t>
   </si>
   <si>
-    <t>Irvin Roob</t>
-  </si>
-  <si>
-    <t>Legacy Sales Planner</t>
-  </si>
-  <si>
-    <t>Blythe Dare</t>
-  </si>
-  <si>
-    <t>National Legal Supervisor</t>
-  </si>
-  <si>
-    <t>Mrs. Rudolph Dach</t>
-  </si>
-  <si>
-    <t>Human Real-Estate Architect</t>
-  </si>
-  <si>
-    <t>Dr. Pearlie Feil</t>
-  </si>
-  <si>
-    <t>District Developer</t>
-  </si>
-  <si>
-    <t>Andrea Pagac</t>
-  </si>
-  <si>
-    <t>Dynamic Consulting Executive</t>
-  </si>
-  <si>
-    <t>Dr. Melida Herzog</t>
-  </si>
-  <si>
-    <t>Hospitality Planner</t>
-  </si>
-  <si>
-    <t>Roger Heaney</t>
-  </si>
-  <si>
-    <t>Advertising Orchestrator</t>
-  </si>
-  <si>
-    <t>Ms. Echo Hand</t>
-  </si>
-  <si>
-    <t>Real-Estate Specialist</t>
-  </si>
-  <si>
-    <t>Lucas Casper</t>
-  </si>
-  <si>
-    <t>Education Administrator</t>
-  </si>
-  <si>
-    <t>Royce Homenick V</t>
-  </si>
-  <si>
-    <t>Design Associate</t>
-  </si>
-  <si>
-    <t>Virgen Renner</t>
-  </si>
-  <si>
-    <t>Dynamic Representative</t>
-  </si>
-  <si>
-    <t>Mr. Chong Dicki</t>
+    <t>Dr. Noe Fisher</t>
+  </si>
+  <si>
+    <t>Sales Supervisor</t>
+  </si>
+  <si>
+    <t>Mrs. Tammie Streich</t>
+  </si>
+  <si>
+    <t>Future Orchestrator</t>
+  </si>
+  <si>
+    <t>Brian Hansen IV</t>
+  </si>
+  <si>
+    <t>Central Healthcare Manager</t>
+  </si>
+  <si>
+    <t>Ha Denesik</t>
+  </si>
+  <si>
+    <t>District Design Officer</t>
+  </si>
+  <si>
+    <t>Waylon Walsh</t>
+  </si>
+  <si>
+    <t>Internal Developer</t>
+  </si>
+  <si>
+    <t>Elicia Kilback</t>
+  </si>
+  <si>
+    <t>Senior Design Strategist</t>
+  </si>
+  <si>
+    <t>Jill Stoltenberg III</t>
+  </si>
+  <si>
+    <t>Product Facilitator</t>
+  </si>
+  <si>
+    <t>Ian Stiedemann</t>
+  </si>
+  <si>
+    <t>Senior Legal Specialist</t>
+  </si>
+  <si>
+    <t>Elease Windler</t>
+  </si>
+  <si>
+    <t>Corporate Farming Agent</t>
+  </si>
+  <si>
+    <t>Joel Hickle</t>
+  </si>
+  <si>
+    <t>National Manufacturing Architect</t>
+  </si>
+  <si>
+    <t>Alejandro Jaskolski</t>
+  </si>
+  <si>
+    <t>Community-Services Developer</t>
+  </si>
+  <si>
+    <t>Hermine Waters</t>
+  </si>
+  <si>
+    <t>Government Coordinator</t>
+  </si>
+  <si>
+    <t>Mr. Neda Feest</t>
+  </si>
+  <si>
+    <t>Customer Education Consultant</t>
+  </si>
+  <si>
+    <t>Zackary Tremblay MD</t>
+  </si>
+  <si>
+    <t>Sales Specialist</t>
+  </si>
+  <si>
+    <t>Toby Mann</t>
+  </si>
+  <si>
+    <t>Central Agent</t>
+  </si>
+  <si>
+    <t>Zelda Kuvalis</t>
+  </si>
+  <si>
+    <t>Regional Marketing Strategist</t>
+  </si>
+  <si>
+    <t>Ali O'Connell</t>
+  </si>
+  <si>
+    <t>Regional Accounting Producer</t>
+  </si>
+  <si>
+    <t>Winford Kutch</t>
+  </si>
+  <si>
+    <t>Cedrick Okuneva</t>
   </si>
   <si>
     <t>Community-Services Executive</t>
+  </si>
+  <si>
+    <t>Damian Bernhard</t>
+  </si>
+  <si>
+    <t>National Manager</t>
+  </si>
+  <si>
+    <t>Corey Williamson</t>
+  </si>
+  <si>
+    <t>Corporate Sales Specialist</t>
+  </si>
+  <si>
+    <t>Nelson Homenick III</t>
+  </si>
+  <si>
+    <t>Product Architect</t>
+  </si>
+  <si>
+    <t>Asa Effertz DVM</t>
+  </si>
+  <si>
+    <t>Human Agent</t>
+  </si>
+  <si>
+    <t>Tatum Torphy</t>
+  </si>
+  <si>
+    <t>Marketing Representative</t>
+  </si>
+  <si>
+    <t>Silva Zboncak</t>
+  </si>
+  <si>
+    <t>Hospitality Administrator</t>
+  </si>
+  <si>
+    <t>Ms. Argentina Dibbert</t>
+  </si>
+  <si>
+    <t>Human Mining Designer</t>
+  </si>
+  <si>
+    <t>Shala Kirlin</t>
+  </si>
+  <si>
+    <t>Real-Estate Representative</t>
+  </si>
+  <si>
+    <t>Delmer Reichert</t>
+  </si>
+  <si>
+    <t>Global Legal Engineer</t>
+  </si>
+  <si>
+    <t>Ms. Moses Stokes</t>
+  </si>
+  <si>
+    <t>Marketing Manager</t>
+  </si>
+  <si>
+    <t>Dr. Carlita Morissette</t>
+  </si>
+  <si>
+    <t>Mining Administrator</t>
+  </si>
+  <si>
+    <t>Cory Hagenes</t>
+  </si>
+  <si>
+    <t>Design Orchestrator</t>
+  </si>
+  <si>
+    <t>Carmen Beatty</t>
+  </si>
+  <si>
+    <t>Healthcare Strategist</t>
+  </si>
+  <si>
+    <t>Marisol Kovacek</t>
+  </si>
+  <si>
+    <t>Marketing Liaison</t>
+  </si>
+  <si>
+    <t>Amal Rosenbaum III</t>
+  </si>
+  <si>
+    <t>Real-Estate Coordinator</t>
+  </si>
+  <si>
+    <t>Avery Simonis V</t>
+  </si>
+  <si>
+    <t>Mining Architect</t>
+  </si>
+  <si>
+    <t>Maricruz Hammes</t>
+  </si>
+  <si>
+    <t>Legacy Real-Estate Liaison</t>
+  </si>
+  <si>
+    <t>Esteban Brown</t>
+  </si>
+  <si>
+    <t>Senior Executive</t>
+  </si>
+  <si>
+    <t>Rocco Russel DDS</t>
+  </si>
+  <si>
+    <t>Direct IT Agent</t>
+  </si>
+  <si>
+    <t>Mrs. Siobhan Welch</t>
+  </si>
+  <si>
+    <t>Senior Officer</t>
+  </si>
+  <si>
+    <t>Mr. Evette Stiedemann</t>
+  </si>
+  <si>
+    <t>Human Farming Developer</t>
+  </si>
+  <si>
+    <t>Mrs. Enrique Ernser</t>
+  </si>
+  <si>
+    <t>Francene Mueller</t>
+  </si>
+  <si>
+    <t>International Legal Specialist</t>
+  </si>
+  <si>
+    <t>Chong Goldner</t>
+  </si>
+  <si>
+    <t>Global Orchestrator</t>
   </si>
 </sst>
 </file>
@@ -1510,7 +1504,7 @@
         <v>151</v>
       </c>
       <c r="B76" t="s">
-        <v>152</v>
+        <v>126</v>
       </c>
       <c r="C76" t="n" s="2">
         <v>44626.041666666664</v>
@@ -1518,10 +1512,10 @@
     </row>
     <row r="77">
       <c r="A77" t="s">
+        <v>152</v>
+      </c>
+      <c r="B77" t="s">
         <v>153</v>
-      </c>
-      <c r="B77" t="s">
-        <v>154</v>
       </c>
       <c r="C77" t="n" s="2">
         <v>44633.041666666664</v>
@@ -1529,10 +1523,10 @@
     </row>
     <row r="78">
       <c r="A78" t="s">
+        <v>154</v>
+      </c>
+      <c r="B78" t="s">
         <v>155</v>
-      </c>
-      <c r="B78" t="s">
-        <v>156</v>
       </c>
       <c r="C78" t="n" s="2">
         <v>44640.041666666664</v>
@@ -1540,10 +1534,10 @@
     </row>
     <row r="79">
       <c r="A79" t="s">
+        <v>156</v>
+      </c>
+      <c r="B79" t="s">
         <v>157</v>
-      </c>
-      <c r="B79" t="s">
-        <v>158</v>
       </c>
       <c r="C79" t="n" s="2">
         <v>44647.041666666664</v>
@@ -1551,10 +1545,10 @@
     </row>
     <row r="80">
       <c r="A80" t="s">
+        <v>158</v>
+      </c>
+      <c r="B80" t="s">
         <v>159</v>
-      </c>
-      <c r="B80" t="s">
-        <v>160</v>
       </c>
       <c r="C80" t="n" s="2">
         <v>44654.041666666664</v>
@@ -1562,10 +1556,10 @@
     </row>
     <row r="81">
       <c r="A81" t="s">
+        <v>160</v>
+      </c>
+      <c r="B81" t="s">
         <v>161</v>
-      </c>
-      <c r="B81" t="s">
-        <v>162</v>
       </c>
       <c r="C81" t="n" s="2">
         <v>44661.0</v>
@@ -1573,10 +1567,10 @@
     </row>
     <row r="82">
       <c r="A82" t="s">
+        <v>162</v>
+      </c>
+      <c r="B82" t="s">
         <v>163</v>
-      </c>
-      <c r="B82" t="s">
-        <v>164</v>
       </c>
       <c r="C82" t="n" s="2">
         <v>44668.0</v>
@@ -1584,10 +1578,10 @@
     </row>
     <row r="83">
       <c r="A83" t="s">
+        <v>164</v>
+      </c>
+      <c r="B83" t="s">
         <v>165</v>
-      </c>
-      <c r="B83" t="s">
-        <v>166</v>
       </c>
       <c r="C83" t="n" s="2">
         <v>44675.0</v>
@@ -1595,10 +1589,10 @@
     </row>
     <row r="84">
       <c r="A84" t="s">
+        <v>166</v>
+      </c>
+      <c r="B84" t="s">
         <v>167</v>
-      </c>
-      <c r="B84" t="s">
-        <v>168</v>
       </c>
       <c r="C84" t="n" s="2">
         <v>44682.0</v>
@@ -1606,10 +1600,10 @@
     </row>
     <row r="85">
       <c r="A85" t="s">
+        <v>168</v>
+      </c>
+      <c r="B85" t="s">
         <v>169</v>
-      </c>
-      <c r="B85" t="s">
-        <v>170</v>
       </c>
       <c r="C85" t="n" s="2">
         <v>44689.0</v>
@@ -1617,10 +1611,10 @@
     </row>
     <row r="86">
       <c r="A86" t="s">
+        <v>170</v>
+      </c>
+      <c r="B86" t="s">
         <v>171</v>
-      </c>
-      <c r="B86" t="s">
-        <v>172</v>
       </c>
       <c r="C86" t="n" s="2">
         <v>44696.0</v>
@@ -1628,10 +1622,10 @@
     </row>
     <row r="87">
       <c r="A87" t="s">
+        <v>172</v>
+      </c>
+      <c r="B87" t="s">
         <v>173</v>
-      </c>
-      <c r="B87" t="s">
-        <v>174</v>
       </c>
       <c r="C87" t="n" s="2">
         <v>44703.0</v>
@@ -1639,10 +1633,10 @@
     </row>
     <row r="88">
       <c r="A88" t="s">
+        <v>174</v>
+      </c>
+      <c r="B88" t="s">
         <v>175</v>
-      </c>
-      <c r="B88" t="s">
-        <v>176</v>
       </c>
       <c r="C88" t="n" s="2">
         <v>44710.0</v>
@@ -1650,10 +1644,10 @@
     </row>
     <row r="89">
       <c r="A89" t="s">
+        <v>176</v>
+      </c>
+      <c r="B89" t="s">
         <v>177</v>
-      </c>
-      <c r="B89" t="s">
-        <v>178</v>
       </c>
       <c r="C89" t="n" s="2">
         <v>44717.0</v>
@@ -1661,10 +1655,10 @@
     </row>
     <row r="90">
       <c r="A90" t="s">
+        <v>178</v>
+      </c>
+      <c r="B90" t="s">
         <v>179</v>
-      </c>
-      <c r="B90" t="s">
-        <v>180</v>
       </c>
       <c r="C90" t="n" s="2">
         <v>44724.0</v>
@@ -1672,10 +1666,10 @@
     </row>
     <row r="91">
       <c r="A91" t="s">
+        <v>180</v>
+      </c>
+      <c r="B91" t="s">
         <v>181</v>
-      </c>
-      <c r="B91" t="s">
-        <v>182</v>
       </c>
       <c r="C91" t="n" s="2">
         <v>44731.0</v>
@@ -1683,10 +1677,10 @@
     </row>
     <row r="92">
       <c r="A92" t="s">
+        <v>182</v>
+      </c>
+      <c r="B92" t="s">
         <v>183</v>
-      </c>
-      <c r="B92" t="s">
-        <v>184</v>
       </c>
       <c r="C92" t="n" s="2">
         <v>44738.0</v>
@@ -1694,10 +1688,10 @@
     </row>
     <row r="93">
       <c r="A93" t="s">
+        <v>184</v>
+      </c>
+      <c r="B93" t="s">
         <v>185</v>
-      </c>
-      <c r="B93" t="s">
-        <v>186</v>
       </c>
       <c r="C93" t="n" s="2">
         <v>44745.0</v>
@@ -1705,10 +1699,10 @@
     </row>
     <row r="94">
       <c r="A94" t="s">
+        <v>186</v>
+      </c>
+      <c r="B94" t="s">
         <v>187</v>
-      </c>
-      <c r="B94" t="s">
-        <v>188</v>
       </c>
       <c r="C94" t="n" s="2">
         <v>44752.0</v>
@@ -1716,10 +1710,10 @@
     </row>
     <row r="95">
       <c r="A95" t="s">
+        <v>188</v>
+      </c>
+      <c r="B95" t="s">
         <v>189</v>
-      </c>
-      <c r="B95" t="s">
-        <v>190</v>
       </c>
       <c r="C95" t="n" s="2">
         <v>44759.0</v>
@@ -1727,10 +1721,10 @@
     </row>
     <row r="96">
       <c r="A96" t="s">
+        <v>190</v>
+      </c>
+      <c r="B96" t="s">
         <v>191</v>
-      </c>
-      <c r="B96" t="s">
-        <v>192</v>
       </c>
       <c r="C96" t="n" s="2">
         <v>44766.0</v>
@@ -1738,10 +1732,10 @@
     </row>
     <row r="97">
       <c r="A97" t="s">
+        <v>192</v>
+      </c>
+      <c r="B97" t="s">
         <v>193</v>
-      </c>
-      <c r="B97" t="s">
-        <v>194</v>
       </c>
       <c r="C97" t="n" s="2">
         <v>44773.0</v>
@@ -1749,10 +1743,10 @@
     </row>
     <row r="98">
       <c r="A98" t="s">
+        <v>194</v>
+      </c>
+      <c r="B98" t="s">
         <v>195</v>
-      </c>
-      <c r="B98" t="s">
-        <v>196</v>
       </c>
       <c r="C98" t="n" s="2">
         <v>44780.0</v>
@@ -1760,10 +1754,10 @@
     </row>
     <row r="99">
       <c r="A99" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B99" t="s">
-        <v>198</v>
+        <v>173</v>
       </c>
       <c r="C99" t="n" s="2">
         <v>44787.0</v>
@@ -1771,10 +1765,10 @@
     </row>
     <row r="100">
       <c r="A100" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B100" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C100" t="n" s="2">
         <v>44794.0</v>
@@ -1782,10 +1776,10 @@
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B101" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C101" t="n" s="2">
         <v>44801.0</v>

</xml_diff>

<commit_message>
fix the artifact name
</commit_message>
<xml_diff>
--- a/output/fluentmanyrows.xlsx
+++ b/output/fluentmanyrows.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="202">
   <si>
     <t>Name</t>
   </si>
@@ -23,598 +23,601 @@
     <t>Hired</t>
   </si>
   <si>
-    <t>Miss Bert Quitzon</t>
-  </si>
-  <si>
-    <t>Retail Producer</t>
-  </si>
-  <si>
-    <t>Grace Stamm</t>
-  </si>
-  <si>
-    <t>Investor Real-Estate Specialist</t>
-  </si>
-  <si>
-    <t>Arnoldo Schumm III</t>
-  </si>
-  <si>
-    <t>Internal Consulting Architect</t>
-  </si>
-  <si>
-    <t>Hiram Swift</t>
-  </si>
-  <si>
-    <t>Consulting Assistant</t>
-  </si>
-  <si>
-    <t>Gwen McLaughlin I</t>
-  </si>
-  <si>
-    <t>Accounting Representative</t>
-  </si>
-  <si>
-    <t>Felice Weimann</t>
-  </si>
-  <si>
-    <t>National Liaison</t>
-  </si>
-  <si>
-    <t>Nannie Hamill</t>
-  </si>
-  <si>
-    <t>Legacy Retail Orchestrator</t>
-  </si>
-  <si>
-    <t>Ms. Burt Osinski</t>
-  </si>
-  <si>
-    <t>Regional Real-Estate Agent</t>
-  </si>
-  <si>
-    <t>Sang Friesen</t>
-  </si>
-  <si>
-    <t>Education Analyst</t>
-  </si>
-  <si>
-    <t>Dr. Elvin Kunze</t>
-  </si>
-  <si>
-    <t>Human Education Analyst</t>
-  </si>
-  <si>
-    <t>Malcolm Buckridge</t>
-  </si>
-  <si>
-    <t>Customer Consulting Supervisor</t>
-  </si>
-  <si>
-    <t>Louise Kihn</t>
-  </si>
-  <si>
-    <t>National Farming Manager</t>
-  </si>
-  <si>
-    <t>Miss Louella Parker</t>
-  </si>
-  <si>
-    <t>Hospitality Engineer</t>
-  </si>
-  <si>
-    <t>Mr. Larissa Stroman</t>
-  </si>
-  <si>
-    <t>National Education Designer</t>
-  </si>
-  <si>
-    <t>Kris Kemmer</t>
-  </si>
-  <si>
-    <t>Consulting Facilitator</t>
-  </si>
-  <si>
-    <t>Ezra Goodwin</t>
-  </si>
-  <si>
-    <t>Investor Technology Supervisor</t>
-  </si>
-  <si>
-    <t>Garry Gulgowski</t>
-  </si>
-  <si>
-    <t>Government Orchestrator</t>
-  </si>
-  <si>
-    <t>Marybelle Trantow</t>
-  </si>
-  <si>
-    <t>Internal Real-Estate Administrator</t>
-  </si>
-  <si>
-    <t>Delma Beahan</t>
-  </si>
-  <si>
-    <t>Manufacturing Developer</t>
-  </si>
-  <si>
-    <t>Griselda Wolf</t>
-  </si>
-  <si>
-    <t>Global Officer</t>
-  </si>
-  <si>
-    <t>Kenna Schmitt</t>
-  </si>
-  <si>
-    <t>Product Associate</t>
-  </si>
-  <si>
-    <t>Wilber DuBuque</t>
-  </si>
-  <si>
-    <t>Product Education Specialist</t>
-  </si>
-  <si>
-    <t>Kam Bailey</t>
-  </si>
-  <si>
-    <t>Hospitality Associate</t>
-  </si>
-  <si>
-    <t>Jackson Walter</t>
-  </si>
-  <si>
-    <t>Design Analyst</t>
-  </si>
-  <si>
-    <t>Mrs. Reita Rowe</t>
-  </si>
-  <si>
-    <t>Advertising Assistant</t>
-  </si>
-  <si>
-    <t>Berta Quigley</t>
-  </si>
-  <si>
-    <t>Community-Services Supervisor</t>
-  </si>
-  <si>
-    <t>Cleveland Volkman</t>
-  </si>
-  <si>
-    <t>Design Coordinator</t>
-  </si>
-  <si>
-    <t>Ria Schowalter PhD</t>
-  </si>
-  <si>
-    <t>Forward Assistant</t>
-  </si>
-  <si>
-    <t>Annmarie Buckridge I</t>
-  </si>
-  <si>
-    <t>Legal Developer</t>
-  </si>
-  <si>
-    <t>Francisco Hettinger</t>
-  </si>
-  <si>
-    <t>Education Strategist</t>
-  </si>
-  <si>
-    <t>Louise Corwin V</t>
-  </si>
-  <si>
-    <t>Mining Analyst</t>
-  </si>
-  <si>
-    <t>Gavin Ward</t>
-  </si>
-  <si>
-    <t>Customer Marketing Developer</t>
-  </si>
-  <si>
-    <t>Denver Schroeder</t>
-  </si>
-  <si>
-    <t>Manufacturing Engineer</t>
-  </si>
-  <si>
-    <t>Lawerence Hoppe</t>
-  </si>
-  <si>
-    <t>Technology Architect</t>
-  </si>
-  <si>
-    <t>Lakeesha Jacobson</t>
-  </si>
-  <si>
-    <t>Direct Developer</t>
-  </si>
-  <si>
-    <t>Augustine O'Hara MD</t>
-  </si>
-  <si>
-    <t>Mining Specialist</t>
-  </si>
-  <si>
-    <t>Jacki Harvey III</t>
-  </si>
-  <si>
-    <t>Forward Developer</t>
-  </si>
-  <si>
-    <t>Tomika Kohler Jr.</t>
-  </si>
-  <si>
-    <t>Senior Consulting Orchestrator</t>
-  </si>
-  <si>
-    <t>Chung Bahringer DDS</t>
-  </si>
-  <si>
-    <t>Customer IT Specialist</t>
-  </si>
-  <si>
-    <t>Miss Tommie Fadel</t>
-  </si>
-  <si>
-    <t>Administration Specialist</t>
-  </si>
-  <si>
-    <t>Ezekiel Funk</t>
-  </si>
-  <si>
-    <t>Internal Accounting Strategist</t>
-  </si>
-  <si>
-    <t>Hilma Wolff</t>
-  </si>
-  <si>
-    <t>Customer Mining Technician</t>
-  </si>
-  <si>
-    <t>Stacy Medhurst IV</t>
-  </si>
-  <si>
-    <t>Corporate Administration Assistant</t>
-  </si>
-  <si>
-    <t>Miss Demarcus Schimmel</t>
-  </si>
-  <si>
-    <t>Hospitality Strategist</t>
-  </si>
-  <si>
-    <t>Jules Muller</t>
-  </si>
-  <si>
-    <t>Administration Representative</t>
-  </si>
-  <si>
-    <t>Mr. Michel Rath</t>
-  </si>
-  <si>
-    <t>Consulting Designer</t>
-  </si>
-  <si>
-    <t>Mrs. Maire Harber</t>
-  </si>
-  <si>
-    <t>Design Planner</t>
-  </si>
-  <si>
-    <t>Albertha Marvin</t>
-  </si>
-  <si>
-    <t>Healthcare Specialist</t>
-  </si>
-  <si>
-    <t>Mrs. Lawanna Glover</t>
-  </si>
-  <si>
-    <t>Investor Strategist</t>
-  </si>
-  <si>
-    <t>Steve Hessel</t>
-  </si>
-  <si>
-    <t>Corporate Government Analyst</t>
-  </si>
-  <si>
-    <t>Alejandro Gislason</t>
-  </si>
-  <si>
-    <t>Chief Coordinator</t>
-  </si>
-  <si>
-    <t>Carol Kshlerin IV</t>
-  </si>
-  <si>
-    <t>Chief Farming Technician</t>
-  </si>
-  <si>
-    <t>Pedro Bruen</t>
-  </si>
-  <si>
-    <t>Future Healthcare Orchestrator</t>
-  </si>
-  <si>
-    <t>Julian Christiansen III</t>
-  </si>
-  <si>
-    <t>Regional Administration Supervisor</t>
-  </si>
-  <si>
-    <t>Janina Rodriguez</t>
-  </si>
-  <si>
-    <t>Product Consulting Executive</t>
-  </si>
-  <si>
-    <t>Aretha Zulauf I</t>
-  </si>
-  <si>
-    <t>Legal Producer</t>
-  </si>
-  <si>
-    <t>Dr. Evonne Thompson</t>
+    <t>Janiece Nader</t>
+  </si>
+  <si>
+    <t>Product Planner</t>
+  </si>
+  <si>
+    <t>Kelley Sporer</t>
+  </si>
+  <si>
+    <t>Farming Administrator</t>
+  </si>
+  <si>
+    <t>Tanna Ritchie Jr.</t>
+  </si>
+  <si>
+    <t>Human Orchestrator</t>
+  </si>
+  <si>
+    <t>Paige Stokes I</t>
+  </si>
+  <si>
+    <t>Marketing Director</t>
+  </si>
+  <si>
+    <t>Rosendo Russel Sr.</t>
+  </si>
+  <si>
+    <t>Legal Coordinator</t>
+  </si>
+  <si>
+    <t>Melda Christiansen MD</t>
+  </si>
+  <si>
+    <t>Central Government Coordinator</t>
+  </si>
+  <si>
+    <t>Sharolyn Rau</t>
+  </si>
+  <si>
+    <t>District Education Manager</t>
+  </si>
+  <si>
+    <t>Marshall Kozey</t>
+  </si>
+  <si>
+    <t>National Supervisor</t>
+  </si>
+  <si>
+    <t>Darrick Heidenreich</t>
+  </si>
+  <si>
+    <t>Principal Orchestrator</t>
+  </si>
+  <si>
+    <t>Zack Huel</t>
+  </si>
+  <si>
+    <t>Dynamic Healthcare Facilitator</t>
+  </si>
+  <si>
+    <t>Hugo Balistreri</t>
+  </si>
+  <si>
+    <t>Corporate Director</t>
+  </si>
+  <si>
+    <t>Mrs. Clayton Schaden</t>
+  </si>
+  <si>
+    <t>Product Technician</t>
+  </si>
+  <si>
+    <t>Miss Gayla Wuckert</t>
+  </si>
+  <si>
+    <t>Community-Services Specialist</t>
+  </si>
+  <si>
+    <t>Mr. Ayesha Romaguera</t>
+  </si>
+  <si>
+    <t>Future Representative</t>
+  </si>
+  <si>
+    <t>Kacie Ratke</t>
+  </si>
+  <si>
+    <t>Product Designer</t>
+  </si>
+  <si>
+    <t>Ethan Littel III</t>
+  </si>
+  <si>
+    <t>Central Representative</t>
+  </si>
+  <si>
+    <t>Ernesto Kassulke</t>
+  </si>
+  <si>
+    <t>Banking Planner</t>
+  </si>
+  <si>
+    <t>Tess Jones</t>
+  </si>
+  <si>
+    <t>Dynamic Construction Technician</t>
+  </si>
+  <si>
+    <t>Melany Ondricka</t>
+  </si>
+  <si>
+    <t>Investor Manufacturing Associate</t>
+  </si>
+  <si>
+    <t>Ms. Mickey Daniel</t>
+  </si>
+  <si>
+    <t>Global Hospitality Analyst</t>
+  </si>
+  <si>
+    <t>Kasha Turcotte IV</t>
+  </si>
+  <si>
+    <t>Mining Engineer</t>
+  </si>
+  <si>
+    <t>Livia Hagenes</t>
+  </si>
+  <si>
+    <t>Direct Accounting Engineer</t>
+  </si>
+  <si>
+    <t>Masako Balistreri DDS</t>
+  </si>
+  <si>
+    <t>National Technology Analyst</t>
+  </si>
+  <si>
+    <t>Gail Barton</t>
+  </si>
+  <si>
+    <t>Product Consultant</t>
+  </si>
+  <si>
+    <t>Colton Okuneva</t>
+  </si>
+  <si>
+    <t>International Advertising Facilitator</t>
+  </si>
+  <si>
+    <t>Miss Robin O'Conner</t>
+  </si>
+  <si>
+    <t>Accounting Manager</t>
+  </si>
+  <si>
+    <t>Dick Braun</t>
+  </si>
+  <si>
+    <t>Customer Mining Consultant</t>
+  </si>
+  <si>
+    <t>Britt Daugherty II</t>
+  </si>
+  <si>
+    <t>Senior Specialist</t>
+  </si>
+  <si>
+    <t>Shakira Ondricka</t>
+  </si>
+  <si>
+    <t>Manufacturing Specialist</t>
+  </si>
+  <si>
+    <t>Elida Johnston</t>
+  </si>
+  <si>
+    <t>Accounting Assistant</t>
+  </si>
+  <si>
+    <t>Isadora O'Conner MD</t>
+  </si>
+  <si>
+    <t>Direct Legal Executive</t>
+  </si>
+  <si>
+    <t>Dudley Langworth</t>
+  </si>
+  <si>
+    <t>Customer Marketing Supervisor</t>
+  </si>
+  <si>
+    <t>Ashli Harris Jr.</t>
+  </si>
+  <si>
+    <t>Marketing Coordinator</t>
+  </si>
+  <si>
+    <t>Shaun Daniel</t>
+  </si>
+  <si>
+    <t>Lead Hospitality Facilitator</t>
+  </si>
+  <si>
+    <t>Florinda Haley</t>
+  </si>
+  <si>
+    <t>Future Real-Estate Administrator</t>
+  </si>
+  <si>
+    <t>Ross Lockman</t>
+  </si>
+  <si>
+    <t>Future Government Developer</t>
+  </si>
+  <si>
+    <t>Mckinley Rath</t>
+  </si>
+  <si>
+    <t>Forward Accounting Administrator</t>
+  </si>
+  <si>
+    <t>Clementina Reynolds</t>
+  </si>
+  <si>
+    <t>Legacy Consulting Representative</t>
+  </si>
+  <si>
+    <t>Marlon Schoen</t>
+  </si>
+  <si>
+    <t>Community-Services Planner</t>
+  </si>
+  <si>
+    <t>Alena Armstrong</t>
+  </si>
+  <si>
+    <t>Senior Supervisor</t>
+  </si>
+  <si>
+    <t>Petronila Haley</t>
+  </si>
+  <si>
+    <t>Corporate Education Orchestrator</t>
+  </si>
+  <si>
+    <t>Shonna Fay</t>
+  </si>
+  <si>
+    <t>International Manufacturing Agent</t>
+  </si>
+  <si>
+    <t>Cruz Bayer</t>
+  </si>
+  <si>
+    <t>Customer Designer</t>
+  </si>
+  <si>
+    <t>Bobbie Koepp</t>
+  </si>
+  <si>
+    <t>Design Consultant</t>
+  </si>
+  <si>
+    <t>Angelic Kilback</t>
+  </si>
+  <si>
+    <t>Construction Agent</t>
+  </si>
+  <si>
+    <t>Ernest Emard</t>
+  </si>
+  <si>
+    <t>Principal Facilitator</t>
+  </si>
+  <si>
+    <t>Georgina Jacobs</t>
+  </si>
+  <si>
+    <t>Investor Farming Associate</t>
+  </si>
+  <si>
+    <t>Carl O'Kon</t>
+  </si>
+  <si>
+    <t>Marketing Engineer</t>
+  </si>
+  <si>
+    <t>Hildred Bechtelar</t>
+  </si>
+  <si>
+    <t>International Marketing Agent</t>
+  </si>
+  <si>
+    <t>Bob White</t>
+  </si>
+  <si>
+    <t>Principal Consultant</t>
+  </si>
+  <si>
+    <t>Ms. Tawna Cremin</t>
+  </si>
+  <si>
+    <t>Banking Representative</t>
+  </si>
+  <si>
+    <t>Mrs. Broderick Schuppe</t>
+  </si>
+  <si>
+    <t>Future Sales Analyst</t>
+  </si>
+  <si>
+    <t>Hipolito Wilderman</t>
+  </si>
+  <si>
+    <t>Global Legal Coordinator</t>
+  </si>
+  <si>
+    <t>Mr. Samara Hahn</t>
+  </si>
+  <si>
+    <t>Dynamic Legal Executive</t>
+  </si>
+  <si>
+    <t>Herschel Sipes</t>
+  </si>
+  <si>
+    <t>Healthcare Assistant</t>
+  </si>
+  <si>
+    <t>Kirby Hauck</t>
+  </si>
+  <si>
+    <t>International Marketing Supervisor</t>
+  </si>
+  <si>
+    <t>Tarah Krajcik</t>
+  </si>
+  <si>
+    <t>Legacy Marketing Representative</t>
+  </si>
+  <si>
+    <t>Chung Ryan</t>
+  </si>
+  <si>
+    <t>Administration Coordinator</t>
+  </si>
+  <si>
+    <t>Corinna Brown</t>
+  </si>
+  <si>
+    <t>Dynamic Associate</t>
+  </si>
+  <si>
+    <t>Zane Langworth</t>
+  </si>
+  <si>
+    <t>Senior Design Engineer</t>
+  </si>
+  <si>
+    <t>Will Nitzsche</t>
+  </si>
+  <si>
+    <t>Internal Director</t>
+  </si>
+  <si>
+    <t>Wyatt Fahey</t>
+  </si>
+  <si>
+    <t>District Farming Facilitator</t>
+  </si>
+  <si>
+    <t>Suzanna Weimann</t>
+  </si>
+  <si>
+    <t>Manufacturing Coordinator</t>
+  </si>
+  <si>
+    <t>Diamond Satterfield</t>
+  </si>
+  <si>
+    <t>Forward Executive</t>
+  </si>
+  <si>
+    <t>Jamey Brekke</t>
+  </si>
+  <si>
+    <t>Future Government Architect</t>
+  </si>
+  <si>
+    <t>Miss Nathaniel Sipes</t>
+  </si>
+  <si>
+    <t>Customer Assistant</t>
+  </si>
+  <si>
+    <t>Lavern Homenick</t>
+  </si>
+  <si>
+    <t>Chief Mining Planner</t>
+  </si>
+  <si>
+    <t>Dr. Wilfredo Ullrich</t>
+  </si>
+  <si>
+    <t>Future Administration Technician</t>
+  </si>
+  <si>
+    <t>Jared Ullrich</t>
+  </si>
+  <si>
+    <t>Construction Manager</t>
+  </si>
+  <si>
+    <t>Jacinta Hintz</t>
+  </si>
+  <si>
+    <t>Corporate Assistant</t>
+  </si>
+  <si>
+    <t>Alpha O'Hara</t>
+  </si>
+  <si>
+    <t>Regional Construction Strategist</t>
+  </si>
+  <si>
+    <t>Vanda King</t>
+  </si>
+  <si>
+    <t>Banking Supervisor</t>
+  </si>
+  <si>
+    <t>Francis Funk MD</t>
+  </si>
+  <si>
+    <t>Internal Administration Specialist</t>
+  </si>
+  <si>
+    <t>Berenice McCullough IV</t>
+  </si>
+  <si>
+    <t>Human Marketing Analyst</t>
+  </si>
+  <si>
+    <t>Donnie Ortiz</t>
+  </si>
+  <si>
+    <t>Customer Hospitality Consultant</t>
+  </si>
+  <si>
+    <t>Nakisha Deckow</t>
+  </si>
+  <si>
+    <t>Healthcare Coordinator</t>
+  </si>
+  <si>
+    <t>Kym Spencer</t>
+  </si>
+  <si>
+    <t>Senior Mining Supervisor</t>
+  </si>
+  <si>
+    <t>Arlean Erdman</t>
+  </si>
+  <si>
+    <t>Design Administrator</t>
+  </si>
+  <si>
+    <t>Les Hilll</t>
+  </si>
+  <si>
+    <t>Direct Banking Officer</t>
+  </si>
+  <si>
+    <t>Delmar Quigley</t>
+  </si>
+  <si>
+    <t>International Advertising Manager</t>
+  </si>
+  <si>
+    <t>Mr. Sigrid West</t>
+  </si>
+  <si>
+    <t>Marcellus Trantow</t>
+  </si>
+  <si>
+    <t>Chief Planner</t>
+  </si>
+  <si>
+    <t>Mrs. Darby Bartoletti</t>
+  </si>
+  <si>
+    <t>Internal Advertising Designer</t>
+  </si>
+  <si>
+    <t>Elise Hartmann PhD</t>
+  </si>
+  <si>
+    <t>Lead Banking Liaison</t>
+  </si>
+  <si>
+    <t>Myrle Ritchie</t>
+  </si>
+  <si>
+    <t>Advertising Director</t>
+  </si>
+  <si>
+    <t>Jackie Jenkins</t>
+  </si>
+  <si>
+    <t>Marketing Administrator</t>
+  </si>
+  <si>
+    <t>Huey Heller</t>
+  </si>
+  <si>
+    <t>Human Assistant</t>
+  </si>
+  <si>
+    <t>Bibi Hauck</t>
+  </si>
+  <si>
+    <t>Real-Estate Orchestrator</t>
+  </si>
+  <si>
+    <t>Ozzie Ritchie</t>
   </si>
   <si>
     <t>Farming Analyst</t>
   </si>
   <si>
-    <t>Dr. Noe Fisher</t>
-  </si>
-  <si>
-    <t>Sales Supervisor</t>
-  </si>
-  <si>
-    <t>Mrs. Tammie Streich</t>
-  </si>
-  <si>
-    <t>Future Orchestrator</t>
-  </si>
-  <si>
-    <t>Brian Hansen IV</t>
-  </si>
-  <si>
-    <t>Central Healthcare Manager</t>
-  </si>
-  <si>
-    <t>Ha Denesik</t>
-  </si>
-  <si>
-    <t>District Design Officer</t>
-  </si>
-  <si>
-    <t>Waylon Walsh</t>
-  </si>
-  <si>
-    <t>Internal Developer</t>
-  </si>
-  <si>
-    <t>Elicia Kilback</t>
-  </si>
-  <si>
-    <t>Senior Design Strategist</t>
-  </si>
-  <si>
-    <t>Jill Stoltenberg III</t>
-  </si>
-  <si>
-    <t>Product Facilitator</t>
-  </si>
-  <si>
-    <t>Ian Stiedemann</t>
-  </si>
-  <si>
-    <t>Senior Legal Specialist</t>
-  </si>
-  <si>
-    <t>Elease Windler</t>
-  </si>
-  <si>
-    <t>Corporate Farming Agent</t>
-  </si>
-  <si>
-    <t>Joel Hickle</t>
-  </si>
-  <si>
-    <t>National Manufacturing Architect</t>
-  </si>
-  <si>
-    <t>Alejandro Jaskolski</t>
-  </si>
-  <si>
-    <t>Community-Services Developer</t>
-  </si>
-  <si>
-    <t>Hermine Waters</t>
-  </si>
-  <si>
-    <t>Government Coordinator</t>
-  </si>
-  <si>
-    <t>Mr. Neda Feest</t>
-  </si>
-  <si>
-    <t>Customer Education Consultant</t>
-  </si>
-  <si>
-    <t>Zackary Tremblay MD</t>
-  </si>
-  <si>
-    <t>Sales Specialist</t>
-  </si>
-  <si>
-    <t>Toby Mann</t>
-  </si>
-  <si>
-    <t>Central Agent</t>
-  </si>
-  <si>
-    <t>Zelda Kuvalis</t>
-  </si>
-  <si>
-    <t>Regional Marketing Strategist</t>
-  </si>
-  <si>
-    <t>Ali O'Connell</t>
-  </si>
-  <si>
-    <t>Regional Accounting Producer</t>
-  </si>
-  <si>
-    <t>Winford Kutch</t>
-  </si>
-  <si>
-    <t>Cedrick Okuneva</t>
-  </si>
-  <si>
-    <t>Community-Services Executive</t>
-  </si>
-  <si>
-    <t>Damian Bernhard</t>
-  </si>
-  <si>
-    <t>National Manager</t>
-  </si>
-  <si>
-    <t>Corey Williamson</t>
-  </si>
-  <si>
-    <t>Corporate Sales Specialist</t>
-  </si>
-  <si>
-    <t>Nelson Homenick III</t>
-  </si>
-  <si>
-    <t>Product Architect</t>
-  </si>
-  <si>
-    <t>Asa Effertz DVM</t>
-  </si>
-  <si>
-    <t>Human Agent</t>
-  </si>
-  <si>
-    <t>Tatum Torphy</t>
-  </si>
-  <si>
-    <t>Marketing Representative</t>
-  </si>
-  <si>
-    <t>Silva Zboncak</t>
-  </si>
-  <si>
-    <t>Hospitality Administrator</t>
-  </si>
-  <si>
-    <t>Ms. Argentina Dibbert</t>
-  </si>
-  <si>
-    <t>Human Mining Designer</t>
-  </si>
-  <si>
-    <t>Shala Kirlin</t>
-  </si>
-  <si>
-    <t>Real-Estate Representative</t>
-  </si>
-  <si>
-    <t>Delmer Reichert</t>
-  </si>
-  <si>
-    <t>Global Legal Engineer</t>
-  </si>
-  <si>
-    <t>Ms. Moses Stokes</t>
-  </si>
-  <si>
-    <t>Marketing Manager</t>
-  </si>
-  <si>
-    <t>Dr. Carlita Morissette</t>
-  </si>
-  <si>
-    <t>Mining Administrator</t>
-  </si>
-  <si>
-    <t>Cory Hagenes</t>
-  </si>
-  <si>
-    <t>Design Orchestrator</t>
-  </si>
-  <si>
-    <t>Carmen Beatty</t>
-  </si>
-  <si>
-    <t>Healthcare Strategist</t>
-  </si>
-  <si>
-    <t>Marisol Kovacek</t>
-  </si>
-  <si>
-    <t>Marketing Liaison</t>
-  </si>
-  <si>
-    <t>Amal Rosenbaum III</t>
-  </si>
-  <si>
-    <t>Real-Estate Coordinator</t>
-  </si>
-  <si>
-    <t>Avery Simonis V</t>
-  </si>
-  <si>
-    <t>Mining Architect</t>
-  </si>
-  <si>
-    <t>Maricruz Hammes</t>
-  </si>
-  <si>
-    <t>Legacy Real-Estate Liaison</t>
-  </si>
-  <si>
-    <t>Esteban Brown</t>
-  </si>
-  <si>
-    <t>Senior Executive</t>
-  </si>
-  <si>
-    <t>Rocco Russel DDS</t>
-  </si>
-  <si>
-    <t>Direct IT Agent</t>
-  </si>
-  <si>
-    <t>Mrs. Siobhan Welch</t>
-  </si>
-  <si>
-    <t>Senior Officer</t>
-  </si>
-  <si>
-    <t>Mr. Evette Stiedemann</t>
-  </si>
-  <si>
-    <t>Human Farming Developer</t>
-  </si>
-  <si>
-    <t>Mrs. Enrique Ernser</t>
-  </si>
-  <si>
-    <t>Francene Mueller</t>
-  </si>
-  <si>
-    <t>International Legal Specialist</t>
-  </si>
-  <si>
-    <t>Chong Goldner</t>
-  </si>
-  <si>
-    <t>Global Orchestrator</t>
+    <t>Zella Grady</t>
+  </si>
+  <si>
+    <t>Community-Services Liaison</t>
+  </si>
+  <si>
+    <t>Mr. Ezra Baumbach</t>
+  </si>
+  <si>
+    <t>Lead Accounting Liaison</t>
+  </si>
+  <si>
+    <t>Miss Stuart Gutkowski</t>
+  </si>
+  <si>
+    <t>Mining Executive</t>
+  </si>
+  <si>
+    <t>Ervin Luettgen</t>
+  </si>
+  <si>
+    <t>IT Associate</t>
+  </si>
+  <si>
+    <t>Tanika Jacobson</t>
+  </si>
+  <si>
+    <t>Customer Community-Services Coordinator</t>
+  </si>
+  <si>
+    <t>Miss Breanna Marvin</t>
+  </si>
+  <si>
+    <t>Corporate Producer</t>
+  </si>
+  <si>
+    <t>Sally Haag</t>
+  </si>
+  <si>
+    <t>Direct Orchestrator</t>
+  </si>
+  <si>
+    <t>Amos Daniel III</t>
+  </si>
+  <si>
+    <t>Accounting Consultant</t>
+  </si>
+  <si>
+    <t>Mr. Kurt Feil</t>
+  </si>
+  <si>
+    <t>Hospitality Director</t>
+  </si>
+  <si>
+    <t>Gale Altenwerth</t>
+  </si>
+  <si>
+    <t>Human Marketing Officer</t>
+  </si>
+  <si>
+    <t>Angelique Kreiger</t>
+  </si>
+  <si>
+    <t>Lead Banking Facilitator</t>
   </si>
 </sst>
 </file>
@@ -1504,7 +1507,7 @@
         <v>151</v>
       </c>
       <c r="B76" t="s">
-        <v>126</v>
+        <v>152</v>
       </c>
       <c r="C76" t="n" s="2">
         <v>44626.041666666664</v>
@@ -1512,10 +1515,10 @@
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B77" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C77" t="n" s="2">
         <v>44633.041666666664</v>
@@ -1523,10 +1526,10 @@
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B78" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C78" t="n" s="2">
         <v>44640.041666666664</v>
@@ -1534,10 +1537,10 @@
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B79" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C79" t="n" s="2">
         <v>44647.041666666664</v>
@@ -1545,10 +1548,10 @@
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B80" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C80" t="n" s="2">
         <v>44654.041666666664</v>
@@ -1556,10 +1559,10 @@
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B81" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C81" t="n" s="2">
         <v>44661.0</v>
@@ -1567,10 +1570,10 @@
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B82" t="s">
-        <v>163</v>
+        <v>28</v>
       </c>
       <c r="C82" t="n" s="2">
         <v>44668.0</v>
@@ -1757,7 +1760,7 @@
         <v>196</v>
       </c>
       <c r="B99" t="s">
-        <v>173</v>
+        <v>197</v>
       </c>
       <c r="C99" t="n" s="2">
         <v>44787.0</v>
@@ -1765,10 +1768,10 @@
     </row>
     <row r="100">
       <c r="A100" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B100" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C100" t="n" s="2">
         <v>44794.0</v>
@@ -1776,10 +1779,10 @@
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B101" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C101" t="n" s="2">
         <v>44801.0</v>

</xml_diff>